<commit_message>
V 2.1 DB-DB、DB-HUDI;use Scala Script load HDFS Data to Hudi,support mor、cow.
</commit_message>
<xml_diff>
--- a/OtherInformation/Data Fabric CDC Init (DB-DB) 性能测试结果.xlsx
+++ b/OtherInformation/Data Fabric CDC Init (DB-DB) 性能测试结果.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SoftWare\A_WORK\IDEA-workspace\boraydata-demo\TableCloneManage\相关资料\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SoftWare\A_WORK\IDEA-workspace\boraydata-demo\TableCloneManage\OtherInformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F66FB0-9452-428F-8F88-1297B08AA114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FD0694-75F3-4D93-9313-CA8C99E8CA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="201">
   <si>
     <t>获取Source端的表信息</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -864,12 +865,180 @@
     <t>仅仅是将A表的数据插入到B表中。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>DB-DB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB-Hudi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDC Init</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MySQL-Hudi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PgSQL-Hudi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4min</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4min30s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>parallelism:40</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Driver:       cores:1    memory:4GB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Executor:   num:10    cores:2   memory:4GB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spark (Spark2 on yarn) 运行作业相关参数</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spark (Spark3 on Master) 运行作业相关参数</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Executor:   num:3     cores:8   memory:4GB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>parallelism:60</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>运行作业后集群资源占用  87.3% of Cluster</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>运行作业后集群资源占用  78.3% of Cluster</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>21min41s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">以 TPC-H lineitem 表，数据量为 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SF1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 约（600W）为测试数据</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">以 TPC-H lineitem 表，数据量为 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SF10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 约（6000W）为测试数据</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDC Init工具 以 lineitem_sf1 为参考的性能</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>31s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>65s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>13s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1min 41s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1min 3s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF1 的 DB-DB、DB-Hudi 都是在CDC节点上进行的测试。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF10 的 DB-DB、DB-Hudi 是申请的测试平台进行的测试。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4min3s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4min 52s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4min 35s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1058,6 +1227,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1117,7 +1295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="56">
+  <borders count="61">
     <border>
       <left/>
       <right/>
@@ -1790,6 +1968,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thick">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1825,7 +2056,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1924,6 +2155,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="34" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="34" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2176,6 +2418,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="34" xfId="10" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2209,8 +2454,71 @@
     <xf numFmtId="0" fontId="23" fillId="6" borderId="48" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="34" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="40" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="57" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="42" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="58" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="59" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="60" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="41" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="46" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="47" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="48" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="44" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="56" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -2506,7 +2814,7 @@
   <dimension ref="D1:N19"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:L6"/>
+      <selection activeCell="I7" sqref="I7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.05" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2523,38 +2831,38 @@
     <row r="1" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="59" t="s">
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
     </row>
     <row r="2" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="63" t="s">
+      <c r="G2" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="H2" s="68"/>
+      <c r="I2" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="59" t="s">
+      <c r="J2" s="68"/>
+      <c r="K2" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59" t="s">
+      <c r="L2" s="64"/>
+      <c r="M2" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="59"/>
+      <c r="N2" s="64"/>
     </row>
     <row r="3" spans="5:14" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E3" s="2" t="s">
@@ -2587,269 +2895,269 @@
       </c>
     </row>
     <row r="4" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="55" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="67" t="s">
+      <c r="H4" s="63"/>
+      <c r="I4" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="58"/>
-      <c r="K4" s="60" t="s">
+      <c r="J4" s="63"/>
+      <c r="K4" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60" t="s">
+      <c r="L4" s="65"/>
+      <c r="M4" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="61"/>
+      <c r="N4" s="66"/>
     </row>
     <row r="5" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="51"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66" t="s">
+      <c r="H5" s="71"/>
+      <c r="I5" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="66"/>
-      <c r="K5" s="53" t="s">
+      <c r="J5" s="71"/>
+      <c r="K5" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53" t="s">
+      <c r="L5" s="58"/>
+      <c r="M5" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="54"/>
+      <c r="N5" s="59"/>
     </row>
     <row r="6" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="51"/>
+      <c r="E6" s="56"/>
       <c r="F6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="65" t="s">
+      <c r="G6" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66" t="s">
+      <c r="H6" s="71"/>
+      <c r="I6" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="66"/>
-      <c r="K6" s="53" t="s">
+      <c r="J6" s="71"/>
+      <c r="K6" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53" t="s">
+      <c r="L6" s="58"/>
+      <c r="M6" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="54"/>
+      <c r="N6" s="59"/>
     </row>
     <row r="7" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="51"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="64" t="s">
+      <c r="G7" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62" t="s">
+      <c r="H7" s="67"/>
+      <c r="I7" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="62"/>
-      <c r="K7" s="55" t="s">
+      <c r="J7" s="67"/>
+      <c r="K7" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55" t="s">
+      <c r="L7" s="60"/>
+      <c r="M7" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="N7" s="56"/>
+      <c r="N7" s="61"/>
     </row>
     <row r="8" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="2"/>
       <c r="F8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="52" t="s">
+      <c r="G8" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52" t="s">
+      <c r="H8" s="57"/>
+      <c r="I8" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52" t="s">
+      <c r="J8" s="57"/>
+      <c r="K8" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52" t="s">
+      <c r="L8" s="57"/>
+      <c r="M8" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="52"/>
+      <c r="N8" s="57"/>
     </row>
     <row r="9" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E9" s="2"/>
       <c r="F9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52" t="s">
+      <c r="H9" s="57"/>
+      <c r="I9" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52" t="s">
+      <c r="J9" s="57"/>
+      <c r="K9" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52" t="s">
+      <c r="L9" s="57"/>
+      <c r="M9" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="52"/>
+      <c r="N9" s="57"/>
     </row>
     <row r="10" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="72" t="s">
+      <c r="E11" s="77" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="71" t="s">
+      <c r="G11" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="71"/>
-      <c r="M11" s="71"/>
-      <c r="N11" s="71"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
     </row>
     <row r="12" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="72"/>
+      <c r="E12" s="77"/>
       <c r="F12" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="71" t="s">
+      <c r="G12" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
-      <c r="N12" s="71"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="76"/>
     </row>
     <row r="13" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="72" t="s">
+      <c r="E13" s="77" t="s">
         <v>48</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="71" t="s">
+      <c r="G13" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="71"/>
-      <c r="K13" s="71"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="71"/>
-      <c r="N13" s="71"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="76"/>
+      <c r="N13" s="76"/>
     </row>
     <row r="14" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="72"/>
+      <c r="E14" s="77"/>
       <c r="F14" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="71" t="s">
+      <c r="G14" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="H14" s="71"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="71"/>
-      <c r="L14" s="71"/>
-      <c r="M14" s="71"/>
-      <c r="N14" s="71"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="76"/>
+      <c r="L14" s="76"/>
+      <c r="M14" s="76"/>
+      <c r="N14" s="76"/>
     </row>
     <row r="15" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E15" s="73" t="s">
+      <c r="E15" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="73"/>
-      <c r="G15" s="74" t="s">
+      <c r="F15" s="78"/>
+      <c r="G15" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="74"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="74"/>
-      <c r="N15" s="74"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="79"/>
     </row>
     <row r="16" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="68" t="s">
+      <c r="E16" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="68"/>
-      <c r="G16" s="74" t="s">
+      <c r="F16" s="73"/>
+      <c r="G16" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="74"/>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="74"/>
-      <c r="L16" s="74"/>
-      <c r="M16" s="74"/>
-      <c r="N16" s="74"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="79"/>
+      <c r="N16" s="79"/>
     </row>
     <row r="17" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="69" t="s">
+      <c r="E17" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="69"/>
-      <c r="G17" s="74" t="s">
+      <c r="F17" s="74"/>
+      <c r="G17" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="74"/>
-      <c r="L17" s="74"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="74"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="79"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="79"/>
     </row>
     <row r="18" spans="5:14" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="70" t="s">
+      <c r="E18" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="70"/>
-      <c r="M18" s="70"/>
-      <c r="N18" s="70"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="75"/>
+      <c r="M18" s="75"/>
+      <c r="N18" s="75"/>
     </row>
     <row r="19" spans="5:14" ht="28.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2930,50 +3238,50 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:38" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="101" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="96"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
-      <c r="S5" s="96"/>
-      <c r="T5" s="96"/>
-      <c r="U5" s="96"/>
-      <c r="V5" s="96"/>
-      <c r="W5" s="96"/>
-      <c r="X5" s="96"/>
-      <c r="Y5" s="96"/>
-      <c r="Z5" s="96"/>
-      <c r="AA5" s="96"/>
-      <c r="AB5" s="96"/>
-      <c r="AC5" s="96"/>
-      <c r="AD5" s="96"/>
-      <c r="AE5" s="96"/>
-      <c r="AF5" s="96"/>
-      <c r="AG5" s="96"/>
-      <c r="AH5" s="96"/>
-      <c r="AI5" s="96"/>
-      <c r="AJ5" s="96"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="101"/>
+      <c r="O5" s="101"/>
+      <c r="P5" s="101"/>
+      <c r="Q5" s="101"/>
+      <c r="R5" s="101"/>
+      <c r="S5" s="101"/>
+      <c r="T5" s="101"/>
+      <c r="U5" s="101"/>
+      <c r="V5" s="101"/>
+      <c r="W5" s="101"/>
+      <c r="X5" s="101"/>
+      <c r="Y5" s="101"/>
+      <c r="Z5" s="101"/>
+      <c r="AA5" s="101"/>
+      <c r="AB5" s="101"/>
+      <c r="AC5" s="101"/>
+      <c r="AD5" s="101"/>
+      <c r="AE5" s="101"/>
+      <c r="AF5" s="101"/>
+      <c r="AG5" s="101"/>
+      <c r="AH5" s="101"/>
+      <c r="AI5" s="101"/>
+      <c r="AJ5" s="101"/>
     </row>
     <row r="6" spans="2:38" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="2:38" ht="28.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="122" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="118"/>
+      <c r="C7" s="123"/>
       <c r="D7" s="14" t="s">
         <v>81</v>
       </c>
@@ -3017,146 +3325,146 @@
       <c r="AJ7" s="16"/>
     </row>
     <row r="8" spans="2:38" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="116" t="s">
+      <c r="B8" s="121" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="98"/>
-      <c r="D8" s="98" t="s">
+      <c r="C8" s="103"/>
+      <c r="D8" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="97" t="s">
+      <c r="E8" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="98" t="s">
+      <c r="F8" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="98" t="s">
+      <c r="G8" s="103" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="100" t="s">
+      <c r="H8" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="105" t="s">
+      <c r="I8" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="J8" s="106"/>
-      <c r="K8" s="106"/>
-      <c r="L8" s="106"/>
-      <c r="M8" s="106"/>
-      <c r="N8" s="106"/>
-      <c r="O8" s="106"/>
-      <c r="P8" s="106"/>
-      <c r="Q8" s="106"/>
-      <c r="R8" s="106"/>
-      <c r="S8" s="106"/>
-      <c r="T8" s="106"/>
-      <c r="U8" s="106"/>
-      <c r="V8" s="106"/>
-      <c r="W8" s="106"/>
-      <c r="X8" s="106"/>
-      <c r="Y8" s="106"/>
-      <c r="Z8" s="106"/>
-      <c r="AA8" s="106"/>
-      <c r="AB8" s="106"/>
-      <c r="AC8" s="106"/>
-      <c r="AD8" s="106"/>
-      <c r="AE8" s="106"/>
-      <c r="AF8" s="106"/>
-      <c r="AG8" s="106"/>
-      <c r="AH8" s="106"/>
-      <c r="AI8" s="106"/>
-      <c r="AJ8" s="107"/>
+      <c r="J8" s="111"/>
+      <c r="K8" s="111"/>
+      <c r="L8" s="111"/>
+      <c r="M8" s="111"/>
+      <c r="N8" s="111"/>
+      <c r="O8" s="111"/>
+      <c r="P8" s="111"/>
+      <c r="Q8" s="111"/>
+      <c r="R8" s="111"/>
+      <c r="S8" s="111"/>
+      <c r="T8" s="111"/>
+      <c r="U8" s="111"/>
+      <c r="V8" s="111"/>
+      <c r="W8" s="111"/>
+      <c r="X8" s="111"/>
+      <c r="Y8" s="111"/>
+      <c r="Z8" s="111"/>
+      <c r="AA8" s="111"/>
+      <c r="AB8" s="111"/>
+      <c r="AC8" s="111"/>
+      <c r="AD8" s="111"/>
+      <c r="AE8" s="111"/>
+      <c r="AF8" s="111"/>
+      <c r="AG8" s="111"/>
+      <c r="AH8" s="111"/>
+      <c r="AI8" s="111"/>
+      <c r="AJ8" s="112"/>
       <c r="AK8" s="8"/>
       <c r="AL8" s="8"/>
     </row>
     <row r="9" spans="2:38" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="116"/>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="98"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="102" t="s">
+      <c r="B9" s="121"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="107" t="s">
         <v>63</v>
       </c>
-      <c r="J9" s="103"/>
-      <c r="K9" s="103"/>
-      <c r="L9" s="103"/>
-      <c r="M9" s="103"/>
-      <c r="N9" s="103"/>
-      <c r="O9" s="103"/>
-      <c r="P9" s="103"/>
-      <c r="Q9" s="103"/>
-      <c r="R9" s="103"/>
-      <c r="S9" s="103"/>
-      <c r="T9" s="103"/>
-      <c r="U9" s="103"/>
-      <c r="V9" s="103"/>
-      <c r="W9" s="103"/>
-      <c r="X9" s="103"/>
-      <c r="Y9" s="103"/>
-      <c r="Z9" s="103"/>
-      <c r="AA9" s="103"/>
-      <c r="AB9" s="103"/>
-      <c r="AC9" s="103"/>
-      <c r="AD9" s="103"/>
-      <c r="AE9" s="103"/>
-      <c r="AF9" s="103"/>
-      <c r="AG9" s="103"/>
-      <c r="AH9" s="103"/>
-      <c r="AI9" s="103"/>
-      <c r="AJ9" s="104"/>
+      <c r="J9" s="108"/>
+      <c r="K9" s="108"/>
+      <c r="L9" s="108"/>
+      <c r="M9" s="108"/>
+      <c r="N9" s="108"/>
+      <c r="O9" s="108"/>
+      <c r="P9" s="108"/>
+      <c r="Q9" s="108"/>
+      <c r="R9" s="108"/>
+      <c r="S9" s="108"/>
+      <c r="T9" s="108"/>
+      <c r="U9" s="108"/>
+      <c r="V9" s="108"/>
+      <c r="W9" s="108"/>
+      <c r="X9" s="108"/>
+      <c r="Y9" s="108"/>
+      <c r="Z9" s="108"/>
+      <c r="AA9" s="108"/>
+      <c r="AB9" s="108"/>
+      <c r="AC9" s="108"/>
+      <c r="AD9" s="108"/>
+      <c r="AE9" s="108"/>
+      <c r="AF9" s="108"/>
+      <c r="AG9" s="108"/>
+      <c r="AH9" s="108"/>
+      <c r="AI9" s="108"/>
+      <c r="AJ9" s="109"/>
     </row>
     <row r="10" spans="2:38" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="116"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="98"/>
-      <c r="G10" s="98"/>
-      <c r="H10" s="100"/>
-      <c r="I10" s="112" t="s">
+      <c r="B10" s="121"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="117" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="113"/>
-      <c r="K10" s="113"/>
-      <c r="L10" s="113"/>
-      <c r="M10" s="113"/>
-      <c r="N10" s="113"/>
-      <c r="O10" s="113"/>
-      <c r="P10" s="113"/>
-      <c r="Q10" s="113"/>
-      <c r="R10" s="113"/>
-      <c r="S10" s="114" t="s">
+      <c r="J10" s="118"/>
+      <c r="K10" s="118"/>
+      <c r="L10" s="118"/>
+      <c r="M10" s="118"/>
+      <c r="N10" s="118"/>
+      <c r="O10" s="118"/>
+      <c r="P10" s="118"/>
+      <c r="Q10" s="118"/>
+      <c r="R10" s="118"/>
+      <c r="S10" s="119" t="s">
         <v>79</v>
       </c>
-      <c r="T10" s="114"/>
-      <c r="U10" s="114"/>
-      <c r="V10" s="114"/>
-      <c r="W10" s="114"/>
-      <c r="X10" s="114"/>
-      <c r="Y10" s="114"/>
-      <c r="Z10" s="114"/>
-      <c r="AA10" s="114"/>
-      <c r="AB10" s="114"/>
-      <c r="AC10" s="114"/>
-      <c r="AD10" s="114"/>
-      <c r="AE10" s="114"/>
-      <c r="AF10" s="114"/>
-      <c r="AG10" s="114"/>
-      <c r="AH10" s="114"/>
-      <c r="AI10" s="114"/>
-      <c r="AJ10" s="115"/>
+      <c r="T10" s="119"/>
+      <c r="U10" s="119"/>
+      <c r="V10" s="119"/>
+      <c r="W10" s="119"/>
+      <c r="X10" s="119"/>
+      <c r="Y10" s="119"/>
+      <c r="Z10" s="119"/>
+      <c r="AA10" s="119"/>
+      <c r="AB10" s="119"/>
+      <c r="AC10" s="119"/>
+      <c r="AD10" s="119"/>
+      <c r="AE10" s="119"/>
+      <c r="AF10" s="119"/>
+      <c r="AG10" s="119"/>
+      <c r="AH10" s="119"/>
+      <c r="AI10" s="119"/>
+      <c r="AJ10" s="120"/>
     </row>
     <row r="11" spans="2:38" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="116"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="100"/>
+      <c r="B11" s="121"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="103"/>
+      <c r="F11" s="103"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="105"/>
       <c r="I11" s="25"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
@@ -3187,138 +3495,138 @@
       <c r="AJ11" s="18"/>
     </row>
     <row r="12" spans="2:38" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="116"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="108" t="s">
+      <c r="B12" s="121"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="103"/>
+      <c r="F12" s="113" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="98" t="s">
+      <c r="G12" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="H12" s="111" t="s">
+      <c r="H12" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="105" t="s">
+      <c r="I12" s="110" t="s">
         <v>61</v>
       </c>
-      <c r="J12" s="106"/>
-      <c r="K12" s="106"/>
-      <c r="L12" s="106"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-      <c r="R12" s="106"/>
-      <c r="S12" s="106"/>
-      <c r="T12" s="106"/>
-      <c r="U12" s="106"/>
-      <c r="V12" s="106"/>
-      <c r="W12" s="106"/>
-      <c r="X12" s="106"/>
-      <c r="Y12" s="106"/>
-      <c r="Z12" s="106"/>
-      <c r="AA12" s="106"/>
-      <c r="AB12" s="106"/>
-      <c r="AC12" s="106"/>
-      <c r="AD12" s="106"/>
-      <c r="AE12" s="106"/>
-      <c r="AF12" s="106"/>
-      <c r="AG12" s="106"/>
-      <c r="AH12" s="106"/>
-      <c r="AI12" s="106"/>
-      <c r="AJ12" s="107"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="111"/>
+      <c r="L12" s="111"/>
+      <c r="M12" s="111"/>
+      <c r="N12" s="111"/>
+      <c r="O12" s="111"/>
+      <c r="P12" s="111"/>
+      <c r="Q12" s="111"/>
+      <c r="R12" s="111"/>
+      <c r="S12" s="111"/>
+      <c r="T12" s="111"/>
+      <c r="U12" s="111"/>
+      <c r="V12" s="111"/>
+      <c r="W12" s="111"/>
+      <c r="X12" s="111"/>
+      <c r="Y12" s="111"/>
+      <c r="Z12" s="111"/>
+      <c r="AA12" s="111"/>
+      <c r="AB12" s="111"/>
+      <c r="AC12" s="111"/>
+      <c r="AD12" s="111"/>
+      <c r="AE12" s="111"/>
+      <c r="AF12" s="111"/>
+      <c r="AG12" s="111"/>
+      <c r="AH12" s="111"/>
+      <c r="AI12" s="111"/>
+      <c r="AJ12" s="112"/>
     </row>
     <row r="13" spans="2:38" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="116"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="108"/>
-      <c r="G13" s="98"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="102" t="s">
+      <c r="B13" s="121"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="116"/>
+      <c r="I13" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="J13" s="103"/>
-      <c r="K13" s="103"/>
-      <c r="L13" s="103"/>
-      <c r="M13" s="103"/>
-      <c r="N13" s="103"/>
-      <c r="O13" s="103"/>
-      <c r="P13" s="103"/>
-      <c r="Q13" s="103"/>
-      <c r="R13" s="103"/>
-      <c r="S13" s="103"/>
-      <c r="T13" s="103"/>
-      <c r="U13" s="103"/>
-      <c r="V13" s="103"/>
-      <c r="W13" s="103"/>
-      <c r="X13" s="103"/>
-      <c r="Y13" s="103"/>
-      <c r="Z13" s="103"/>
-      <c r="AA13" s="103"/>
-      <c r="AB13" s="103"/>
-      <c r="AC13" s="103"/>
-      <c r="AD13" s="103"/>
-      <c r="AE13" s="103"/>
-      <c r="AF13" s="103"/>
-      <c r="AG13" s="103"/>
-      <c r="AH13" s="103"/>
-      <c r="AI13" s="103"/>
-      <c r="AJ13" s="104"/>
+      <c r="J13" s="108"/>
+      <c r="K13" s="108"/>
+      <c r="L13" s="108"/>
+      <c r="M13" s="108"/>
+      <c r="N13" s="108"/>
+      <c r="O13" s="108"/>
+      <c r="P13" s="108"/>
+      <c r="Q13" s="108"/>
+      <c r="R13" s="108"/>
+      <c r="S13" s="108"/>
+      <c r="T13" s="108"/>
+      <c r="U13" s="108"/>
+      <c r="V13" s="108"/>
+      <c r="W13" s="108"/>
+      <c r="X13" s="108"/>
+      <c r="Y13" s="108"/>
+      <c r="Z13" s="108"/>
+      <c r="AA13" s="108"/>
+      <c r="AB13" s="108"/>
+      <c r="AC13" s="108"/>
+      <c r="AD13" s="108"/>
+      <c r="AE13" s="108"/>
+      <c r="AF13" s="108"/>
+      <c r="AG13" s="108"/>
+      <c r="AH13" s="108"/>
+      <c r="AI13" s="108"/>
+      <c r="AJ13" s="109"/>
     </row>
     <row r="14" spans="2:38" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="116"/>
-      <c r="C14" s="98"/>
-      <c r="D14" s="98"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="108"/>
-      <c r="G14" s="98"/>
-      <c r="H14" s="111"/>
-      <c r="I14" s="112" t="s">
+      <c r="B14" s="121"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="116"/>
+      <c r="I14" s="117" t="s">
         <v>76</v>
       </c>
-      <c r="J14" s="113"/>
-      <c r="K14" s="113"/>
-      <c r="L14" s="113"/>
-      <c r="M14" s="113"/>
-      <c r="N14" s="113"/>
-      <c r="O14" s="113"/>
-      <c r="P14" s="113"/>
-      <c r="Q14" s="113"/>
-      <c r="R14" s="113"/>
-      <c r="S14" s="114" t="s">
+      <c r="J14" s="118"/>
+      <c r="K14" s="118"/>
+      <c r="L14" s="118"/>
+      <c r="M14" s="118"/>
+      <c r="N14" s="118"/>
+      <c r="O14" s="118"/>
+      <c r="P14" s="118"/>
+      <c r="Q14" s="118"/>
+      <c r="R14" s="118"/>
+      <c r="S14" s="119" t="s">
         <v>78</v>
       </c>
-      <c r="T14" s="114"/>
-      <c r="U14" s="114"/>
-      <c r="V14" s="114"/>
-      <c r="W14" s="114"/>
-      <c r="X14" s="114"/>
-      <c r="Y14" s="114"/>
-      <c r="Z14" s="114"/>
-      <c r="AA14" s="114"/>
-      <c r="AB14" s="114"/>
-      <c r="AC14" s="114"/>
-      <c r="AD14" s="114"/>
-      <c r="AE14" s="114"/>
-      <c r="AF14" s="114"/>
-      <c r="AG14" s="114"/>
-      <c r="AH14" s="114"/>
-      <c r="AI14" s="114"/>
-      <c r="AJ14" s="115"/>
+      <c r="T14" s="119"/>
+      <c r="U14" s="119"/>
+      <c r="V14" s="119"/>
+      <c r="W14" s="119"/>
+      <c r="X14" s="119"/>
+      <c r="Y14" s="119"/>
+      <c r="Z14" s="119"/>
+      <c r="AA14" s="119"/>
+      <c r="AB14" s="119"/>
+      <c r="AC14" s="119"/>
+      <c r="AD14" s="119"/>
+      <c r="AE14" s="119"/>
+      <c r="AF14" s="119"/>
+      <c r="AG14" s="119"/>
+      <c r="AH14" s="119"/>
+      <c r="AI14" s="119"/>
+      <c r="AJ14" s="120"/>
     </row>
     <row r="15" spans="2:38" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="116"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="110"/>
-      <c r="H15" s="111"/>
+      <c r="B15" s="121"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="103"/>
+      <c r="E15" s="103"/>
+      <c r="F15" s="114"/>
+      <c r="G15" s="115"/>
+      <c r="H15" s="116"/>
       <c r="I15" s="26"/>
       <c r="J15" s="23"/>
       <c r="K15" s="23"/>
@@ -3349,105 +3657,105 @@
       <c r="AJ15" s="24"/>
     </row>
     <row r="16" spans="2:38" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="116"/>
-      <c r="C16" s="98"/>
-      <c r="D16" s="98" t="s">
+      <c r="B16" s="121"/>
+      <c r="C16" s="103"/>
+      <c r="D16" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="97" t="s">
+      <c r="E16" s="102" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="98" t="s">
+      <c r="F16" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="98" t="s">
+      <c r="G16" s="103" t="s">
         <v>83</v>
       </c>
-      <c r="H16" s="100" t="s">
+      <c r="H16" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="I16" s="105" t="s">
+      <c r="I16" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="J16" s="106"/>
-      <c r="K16" s="106"/>
-      <c r="L16" s="106"/>
-      <c r="M16" s="106"/>
-      <c r="N16" s="106"/>
-      <c r="O16" s="106"/>
-      <c r="P16" s="106"/>
-      <c r="Q16" s="106"/>
-      <c r="R16" s="106"/>
-      <c r="S16" s="106"/>
-      <c r="T16" s="106"/>
-      <c r="U16" s="106"/>
-      <c r="V16" s="106"/>
-      <c r="W16" s="106"/>
-      <c r="X16" s="106"/>
-      <c r="Y16" s="106"/>
-      <c r="Z16" s="106"/>
-      <c r="AA16" s="106"/>
-      <c r="AB16" s="106"/>
-      <c r="AC16" s="106"/>
-      <c r="AD16" s="106"/>
-      <c r="AE16" s="106"/>
-      <c r="AF16" s="106"/>
-      <c r="AG16" s="106"/>
-      <c r="AH16" s="106"/>
-      <c r="AI16" s="106"/>
-      <c r="AJ16" s="107"/>
+      <c r="J16" s="111"/>
+      <c r="K16" s="111"/>
+      <c r="L16" s="111"/>
+      <c r="M16" s="111"/>
+      <c r="N16" s="111"/>
+      <c r="O16" s="111"/>
+      <c r="P16" s="111"/>
+      <c r="Q16" s="111"/>
+      <c r="R16" s="111"/>
+      <c r="S16" s="111"/>
+      <c r="T16" s="111"/>
+      <c r="U16" s="111"/>
+      <c r="V16" s="111"/>
+      <c r="W16" s="111"/>
+      <c r="X16" s="111"/>
+      <c r="Y16" s="111"/>
+      <c r="Z16" s="111"/>
+      <c r="AA16" s="111"/>
+      <c r="AB16" s="111"/>
+      <c r="AC16" s="111"/>
+      <c r="AD16" s="111"/>
+      <c r="AE16" s="111"/>
+      <c r="AF16" s="111"/>
+      <c r="AG16" s="111"/>
+      <c r="AH16" s="111"/>
+      <c r="AI16" s="111"/>
+      <c r="AJ16" s="112"/>
       <c r="AK16" s="8"/>
       <c r="AL16" s="8"/>
     </row>
     <row r="17" spans="2:45" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="116"/>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98"/>
-      <c r="H17" s="100"/>
-      <c r="I17" s="102" t="s">
+      <c r="B17" s="121"/>
+      <c r="C17" s="103"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="107" t="s">
         <v>96</v>
       </c>
-      <c r="J17" s="103"/>
-      <c r="K17" s="103"/>
-      <c r="L17" s="103"/>
-      <c r="M17" s="103"/>
-      <c r="N17" s="103"/>
-      <c r="O17" s="103"/>
-      <c r="P17" s="103"/>
-      <c r="Q17" s="103"/>
-      <c r="R17" s="103"/>
-      <c r="S17" s="103"/>
-      <c r="T17" s="103"/>
-      <c r="U17" s="103"/>
-      <c r="V17" s="103"/>
-      <c r="W17" s="103"/>
-      <c r="X17" s="103"/>
-      <c r="Y17" s="103"/>
-      <c r="Z17" s="103"/>
-      <c r="AA17" s="103"/>
-      <c r="AB17" s="103"/>
-      <c r="AC17" s="103"/>
-      <c r="AD17" s="103"/>
-      <c r="AE17" s="103"/>
-      <c r="AF17" s="103"/>
-      <c r="AG17" s="103"/>
-      <c r="AH17" s="103"/>
-      <c r="AI17" s="103"/>
-      <c r="AJ17" s="104"/>
+      <c r="J17" s="108"/>
+      <c r="K17" s="108"/>
+      <c r="L17" s="108"/>
+      <c r="M17" s="108"/>
+      <c r="N17" s="108"/>
+      <c r="O17" s="108"/>
+      <c r="P17" s="108"/>
+      <c r="Q17" s="108"/>
+      <c r="R17" s="108"/>
+      <c r="S17" s="108"/>
+      <c r="T17" s="108"/>
+      <c r="U17" s="108"/>
+      <c r="V17" s="108"/>
+      <c r="W17" s="108"/>
+      <c r="X17" s="108"/>
+      <c r="Y17" s="108"/>
+      <c r="Z17" s="108"/>
+      <c r="AA17" s="108"/>
+      <c r="AB17" s="108"/>
+      <c r="AC17" s="108"/>
+      <c r="AD17" s="108"/>
+      <c r="AE17" s="108"/>
+      <c r="AF17" s="108"/>
+      <c r="AG17" s="108"/>
+      <c r="AH17" s="108"/>
+      <c r="AI17" s="108"/>
+      <c r="AJ17" s="109"/>
       <c r="AK17" s="8"/>
       <c r="AL17" s="8"/>
     </row>
     <row r="18" spans="2:45" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="116"/>
-      <c r="C18" s="98"/>
-      <c r="D18" s="98"/>
-      <c r="E18" s="98"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="100"/>
+      <c r="B18" s="121"/>
+      <c r="C18" s="103"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="103"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="105"/>
       <c r="I18" s="27"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
@@ -3480,144 +3788,144 @@
       <c r="AL18" s="8"/>
     </row>
     <row r="19" spans="2:45" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="116"/>
-      <c r="C19" s="98"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98" t="s">
+      <c r="B19" s="121"/>
+      <c r="C19" s="103"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="103"/>
+      <c r="F19" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="98" t="s">
+      <c r="G19" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="H19" s="100" t="s">
+      <c r="H19" s="105" t="s">
         <v>67</v>
       </c>
-      <c r="I19" s="105" t="s">
+      <c r="I19" s="110" t="s">
         <v>72</v>
       </c>
-      <c r="J19" s="106"/>
-      <c r="K19" s="106"/>
-      <c r="L19" s="106"/>
-      <c r="M19" s="106"/>
-      <c r="N19" s="106"/>
-      <c r="O19" s="106"/>
-      <c r="P19" s="106"/>
-      <c r="Q19" s="106"/>
-      <c r="R19" s="106"/>
-      <c r="S19" s="106"/>
-      <c r="T19" s="106"/>
-      <c r="U19" s="106"/>
-      <c r="V19" s="106"/>
-      <c r="W19" s="106"/>
-      <c r="X19" s="106"/>
-      <c r="Y19" s="106"/>
-      <c r="Z19" s="106"/>
-      <c r="AA19" s="106"/>
-      <c r="AB19" s="106"/>
-      <c r="AC19" s="106"/>
-      <c r="AD19" s="106"/>
-      <c r="AE19" s="106"/>
-      <c r="AF19" s="106"/>
-      <c r="AG19" s="106"/>
-      <c r="AH19" s="106"/>
-      <c r="AI19" s="106"/>
-      <c r="AJ19" s="107"/>
+      <c r="J19" s="111"/>
+      <c r="K19" s="111"/>
+      <c r="L19" s="111"/>
+      <c r="M19" s="111"/>
+      <c r="N19" s="111"/>
+      <c r="O19" s="111"/>
+      <c r="P19" s="111"/>
+      <c r="Q19" s="111"/>
+      <c r="R19" s="111"/>
+      <c r="S19" s="111"/>
+      <c r="T19" s="111"/>
+      <c r="U19" s="111"/>
+      <c r="V19" s="111"/>
+      <c r="W19" s="111"/>
+      <c r="X19" s="111"/>
+      <c r="Y19" s="111"/>
+      <c r="Z19" s="111"/>
+      <c r="AA19" s="111"/>
+      <c r="AB19" s="111"/>
+      <c r="AC19" s="111"/>
+      <c r="AD19" s="111"/>
+      <c r="AE19" s="111"/>
+      <c r="AF19" s="111"/>
+      <c r="AG19" s="111"/>
+      <c r="AH19" s="111"/>
+      <c r="AI19" s="111"/>
+      <c r="AJ19" s="112"/>
       <c r="AK19" s="8"/>
       <c r="AL19" s="8"/>
     </row>
     <row r="20" spans="2:45" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="116"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="98"/>
-      <c r="F20" s="98"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="100"/>
-      <c r="I20" s="102" t="s">
+      <c r="B20" s="121"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="103"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="105"/>
+      <c r="I20" s="107" t="s">
         <v>73</v>
       </c>
-      <c r="J20" s="103"/>
-      <c r="K20" s="103"/>
-      <c r="L20" s="103"/>
-      <c r="M20" s="103"/>
-      <c r="N20" s="103"/>
-      <c r="O20" s="103"/>
-      <c r="P20" s="103"/>
-      <c r="Q20" s="103"/>
-      <c r="R20" s="103"/>
-      <c r="S20" s="103"/>
-      <c r="T20" s="103"/>
-      <c r="U20" s="103"/>
-      <c r="V20" s="103"/>
-      <c r="W20" s="103"/>
-      <c r="X20" s="103"/>
-      <c r="Y20" s="103"/>
-      <c r="Z20" s="103"/>
-      <c r="AA20" s="103"/>
-      <c r="AB20" s="103"/>
-      <c r="AC20" s="103"/>
-      <c r="AD20" s="103"/>
-      <c r="AE20" s="103"/>
-      <c r="AF20" s="103"/>
-      <c r="AG20" s="103"/>
-      <c r="AH20" s="103"/>
-      <c r="AI20" s="103"/>
-      <c r="AJ20" s="104"/>
+      <c r="J20" s="108"/>
+      <c r="K20" s="108"/>
+      <c r="L20" s="108"/>
+      <c r="M20" s="108"/>
+      <c r="N20" s="108"/>
+      <c r="O20" s="108"/>
+      <c r="P20" s="108"/>
+      <c r="Q20" s="108"/>
+      <c r="R20" s="108"/>
+      <c r="S20" s="108"/>
+      <c r="T20" s="108"/>
+      <c r="U20" s="108"/>
+      <c r="V20" s="108"/>
+      <c r="W20" s="108"/>
+      <c r="X20" s="108"/>
+      <c r="Y20" s="108"/>
+      <c r="Z20" s="108"/>
+      <c r="AA20" s="108"/>
+      <c r="AB20" s="108"/>
+      <c r="AC20" s="108"/>
+      <c r="AD20" s="108"/>
+      <c r="AE20" s="108"/>
+      <c r="AF20" s="108"/>
+      <c r="AG20" s="108"/>
+      <c r="AH20" s="108"/>
+      <c r="AI20" s="108"/>
+      <c r="AJ20" s="109"/>
       <c r="AK20" s="8"/>
       <c r="AL20" s="8"/>
     </row>
     <row r="21" spans="2:45" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="116"/>
-      <c r="C21" s="98"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="98"/>
-      <c r="F21" s="98"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="100"/>
-      <c r="I21" s="112" t="s">
+      <c r="B21" s="121"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="103"/>
+      <c r="E21" s="103"/>
+      <c r="F21" s="103"/>
+      <c r="G21" s="103"/>
+      <c r="H21" s="105"/>
+      <c r="I21" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="J21" s="113"/>
-      <c r="K21" s="113"/>
-      <c r="L21" s="113"/>
-      <c r="M21" s="113"/>
-      <c r="N21" s="113"/>
-      <c r="O21" s="113"/>
-      <c r="P21" s="113"/>
-      <c r="Q21" s="113"/>
-      <c r="R21" s="113"/>
-      <c r="S21" s="114" t="s">
+      <c r="J21" s="118"/>
+      <c r="K21" s="118"/>
+      <c r="L21" s="118"/>
+      <c r="M21" s="118"/>
+      <c r="N21" s="118"/>
+      <c r="O21" s="118"/>
+      <c r="P21" s="118"/>
+      <c r="Q21" s="118"/>
+      <c r="R21" s="118"/>
+      <c r="S21" s="119" t="s">
         <v>77</v>
       </c>
-      <c r="T21" s="114"/>
-      <c r="U21" s="114"/>
-      <c r="V21" s="114"/>
-      <c r="W21" s="114"/>
-      <c r="X21" s="114"/>
-      <c r="Y21" s="114"/>
-      <c r="Z21" s="114"/>
-      <c r="AA21" s="114"/>
-      <c r="AB21" s="114"/>
-      <c r="AC21" s="114"/>
-      <c r="AD21" s="114"/>
-      <c r="AE21" s="114"/>
-      <c r="AF21" s="114"/>
-      <c r="AG21" s="114"/>
-      <c r="AH21" s="114"/>
-      <c r="AI21" s="114"/>
-      <c r="AJ21" s="115"/>
+      <c r="T21" s="119"/>
+      <c r="U21" s="119"/>
+      <c r="V21" s="119"/>
+      <c r="W21" s="119"/>
+      <c r="X21" s="119"/>
+      <c r="Y21" s="119"/>
+      <c r="Z21" s="119"/>
+      <c r="AA21" s="119"/>
+      <c r="AB21" s="119"/>
+      <c r="AC21" s="119"/>
+      <c r="AD21" s="119"/>
+      <c r="AE21" s="119"/>
+      <c r="AF21" s="119"/>
+      <c r="AG21" s="119"/>
+      <c r="AH21" s="119"/>
+      <c r="AI21" s="119"/>
+      <c r="AJ21" s="120"/>
       <c r="AK21" s="8"/>
       <c r="AL21" s="8"/>
     </row>
     <row r="22" spans="2:45" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="116"/>
-      <c r="C22" s="98"/>
-      <c r="D22" s="98"/>
-      <c r="E22" s="98"/>
-      <c r="F22" s="98"/>
-      <c r="G22" s="98"/>
-      <c r="H22" s="100"/>
+      <c r="B22" s="121"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="103"/>
+      <c r="F22" s="103"/>
+      <c r="G22" s="103"/>
+      <c r="H22" s="105"/>
       <c r="I22" s="25"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -3648,189 +3956,189 @@
       <c r="AJ22" s="18"/>
     </row>
     <row r="23" spans="2:45" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="116"/>
-      <c r="C23" s="98"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="98" t="s">
+      <c r="B23" s="121"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="103"/>
+      <c r="E23" s="103"/>
+      <c r="F23" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="G23" s="98" t="s">
+      <c r="G23" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="H23" s="100" t="s">
+      <c r="H23" s="105" t="s">
         <v>71</v>
       </c>
-      <c r="I23" s="105" t="s">
+      <c r="I23" s="110" t="s">
         <v>60</v>
       </c>
-      <c r="J23" s="106"/>
-      <c r="K23" s="106"/>
-      <c r="L23" s="106"/>
-      <c r="M23" s="106"/>
-      <c r="N23" s="106"/>
-      <c r="O23" s="106"/>
-      <c r="P23" s="106"/>
-      <c r="Q23" s="106"/>
-      <c r="R23" s="106"/>
-      <c r="S23" s="106"/>
-      <c r="T23" s="106"/>
-      <c r="U23" s="106"/>
-      <c r="V23" s="106"/>
-      <c r="W23" s="106"/>
-      <c r="X23" s="106"/>
-      <c r="Y23" s="106"/>
-      <c r="Z23" s="106"/>
-      <c r="AA23" s="106"/>
-      <c r="AB23" s="106"/>
-      <c r="AC23" s="106"/>
-      <c r="AD23" s="106"/>
-      <c r="AE23" s="106"/>
-      <c r="AF23" s="106"/>
-      <c r="AG23" s="106"/>
-      <c r="AH23" s="106"/>
-      <c r="AI23" s="106"/>
-      <c r="AJ23" s="107"/>
+      <c r="J23" s="111"/>
+      <c r="K23" s="111"/>
+      <c r="L23" s="111"/>
+      <c r="M23" s="111"/>
+      <c r="N23" s="111"/>
+      <c r="O23" s="111"/>
+      <c r="P23" s="111"/>
+      <c r="Q23" s="111"/>
+      <c r="R23" s="111"/>
+      <c r="S23" s="111"/>
+      <c r="T23" s="111"/>
+      <c r="U23" s="111"/>
+      <c r="V23" s="111"/>
+      <c r="W23" s="111"/>
+      <c r="X23" s="111"/>
+      <c r="Y23" s="111"/>
+      <c r="Z23" s="111"/>
+      <c r="AA23" s="111"/>
+      <c r="AB23" s="111"/>
+      <c r="AC23" s="111"/>
+      <c r="AD23" s="111"/>
+      <c r="AE23" s="111"/>
+      <c r="AF23" s="111"/>
+      <c r="AG23" s="111"/>
+      <c r="AH23" s="111"/>
+      <c r="AI23" s="111"/>
+      <c r="AJ23" s="112"/>
     </row>
     <row r="24" spans="2:45" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="116"/>
-      <c r="C24" s="98"/>
-      <c r="D24" s="98"/>
-      <c r="E24" s="98"/>
-      <c r="F24" s="98"/>
-      <c r="G24" s="98"/>
-      <c r="H24" s="100"/>
-      <c r="I24" s="102" t="s">
+      <c r="B24" s="121"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="103"/>
+      <c r="E24" s="103"/>
+      <c r="F24" s="103"/>
+      <c r="G24" s="103"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="107" t="s">
         <v>95</v>
       </c>
-      <c r="J24" s="103"/>
-      <c r="K24" s="103"/>
-      <c r="L24" s="103"/>
-      <c r="M24" s="103"/>
-      <c r="N24" s="103"/>
-      <c r="O24" s="103"/>
-      <c r="P24" s="103"/>
-      <c r="Q24" s="103"/>
-      <c r="R24" s="103"/>
-      <c r="S24" s="103"/>
-      <c r="T24" s="103"/>
-      <c r="U24" s="103"/>
-      <c r="V24" s="103"/>
-      <c r="W24" s="103"/>
-      <c r="X24" s="103"/>
-      <c r="Y24" s="103"/>
-      <c r="Z24" s="103"/>
-      <c r="AA24" s="103"/>
-      <c r="AB24" s="103"/>
-      <c r="AC24" s="103"/>
-      <c r="AD24" s="103"/>
-      <c r="AE24" s="103"/>
-      <c r="AF24" s="103"/>
-      <c r="AG24" s="103"/>
-      <c r="AH24" s="103"/>
-      <c r="AI24" s="103"/>
-      <c r="AJ24" s="104"/>
+      <c r="J24" s="108"/>
+      <c r="K24" s="108"/>
+      <c r="L24" s="108"/>
+      <c r="M24" s="108"/>
+      <c r="N24" s="108"/>
+      <c r="O24" s="108"/>
+      <c r="P24" s="108"/>
+      <c r="Q24" s="108"/>
+      <c r="R24" s="108"/>
+      <c r="S24" s="108"/>
+      <c r="T24" s="108"/>
+      <c r="U24" s="108"/>
+      <c r="V24" s="108"/>
+      <c r="W24" s="108"/>
+      <c r="X24" s="108"/>
+      <c r="Y24" s="108"/>
+      <c r="Z24" s="108"/>
+      <c r="AA24" s="108"/>
+      <c r="AB24" s="108"/>
+      <c r="AC24" s="108"/>
+      <c r="AD24" s="108"/>
+      <c r="AE24" s="108"/>
+      <c r="AF24" s="108"/>
+      <c r="AG24" s="108"/>
+      <c r="AH24" s="108"/>
+      <c r="AI24" s="108"/>
+      <c r="AJ24" s="109"/>
     </row>
     <row r="25" spans="2:45" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="93"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="94"/>
-      <c r="F25" s="94"/>
-      <c r="G25" s="94"/>
-      <c r="H25" s="94"/>
-      <c r="I25" s="94"/>
-      <c r="J25" s="94"/>
-      <c r="K25" s="94"/>
-      <c r="L25" s="94"/>
-      <c r="M25" s="94"/>
-      <c r="N25" s="94"/>
-      <c r="O25" s="94"/>
-      <c r="P25" s="94"/>
-      <c r="Q25" s="94"/>
-      <c r="R25" s="94"/>
-      <c r="S25" s="94"/>
-      <c r="T25" s="94"/>
-      <c r="U25" s="94"/>
-      <c r="V25" s="94"/>
-      <c r="W25" s="94"/>
-      <c r="X25" s="94"/>
-      <c r="Y25" s="94"/>
-      <c r="Z25" s="94"/>
-      <c r="AA25" s="94"/>
-      <c r="AB25" s="94"/>
-      <c r="AC25" s="94"/>
-      <c r="AD25" s="94"/>
-      <c r="AE25" s="94"/>
-      <c r="AF25" s="94"/>
-      <c r="AG25" s="94"/>
-      <c r="AH25" s="94"/>
-      <c r="AI25" s="94"/>
-      <c r="AJ25" s="95"/>
+      <c r="B25" s="98"/>
+      <c r="C25" s="99"/>
+      <c r="D25" s="99"/>
+      <c r="E25" s="99"/>
+      <c r="F25" s="99"/>
+      <c r="G25" s="99"/>
+      <c r="H25" s="99"/>
+      <c r="I25" s="99"/>
+      <c r="J25" s="99"/>
+      <c r="K25" s="99"/>
+      <c r="L25" s="99"/>
+      <c r="M25" s="99"/>
+      <c r="N25" s="99"/>
+      <c r="O25" s="99"/>
+      <c r="P25" s="99"/>
+      <c r="Q25" s="99"/>
+      <c r="R25" s="99"/>
+      <c r="S25" s="99"/>
+      <c r="T25" s="99"/>
+      <c r="U25" s="99"/>
+      <c r="V25" s="99"/>
+      <c r="W25" s="99"/>
+      <c r="X25" s="99"/>
+      <c r="Y25" s="99"/>
+      <c r="Z25" s="99"/>
+      <c r="AA25" s="99"/>
+      <c r="AB25" s="99"/>
+      <c r="AC25" s="99"/>
+      <c r="AD25" s="99"/>
+      <c r="AE25" s="99"/>
+      <c r="AF25" s="99"/>
+      <c r="AG25" s="99"/>
+      <c r="AH25" s="99"/>
+      <c r="AI25" s="99"/>
+      <c r="AJ25" s="100"/>
     </row>
     <row r="26" spans="2:45" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="116" t="s">
+      <c r="B26" s="121" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="98"/>
-      <c r="D26" s="98" t="s">
+      <c r="C26" s="103"/>
+      <c r="D26" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="97" t="s">
+      <c r="E26" s="102" t="s">
         <v>92</v>
       </c>
-      <c r="F26" s="98" t="s">
+      <c r="F26" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="G26" s="98" t="s">
+      <c r="G26" s="103" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="100" t="s">
+      <c r="H26" s="105" t="s">
         <v>86</v>
       </c>
-      <c r="I26" s="105" t="s">
+      <c r="I26" s="110" t="s">
         <v>89</v>
       </c>
-      <c r="J26" s="106"/>
-      <c r="K26" s="106"/>
-      <c r="L26" s="106"/>
-      <c r="M26" s="106"/>
-      <c r="N26" s="106"/>
-      <c r="O26" s="106"/>
-      <c r="P26" s="106"/>
-      <c r="Q26" s="106"/>
-      <c r="R26" s="106"/>
-      <c r="S26" s="106"/>
-      <c r="T26" s="106"/>
-      <c r="U26" s="106"/>
-      <c r="V26" s="106"/>
-      <c r="W26" s="106"/>
-      <c r="X26" s="106"/>
-      <c r="Y26" s="106"/>
-      <c r="Z26" s="106"/>
-      <c r="AA26" s="106"/>
-      <c r="AB26" s="106"/>
-      <c r="AC26" s="106"/>
-      <c r="AD26" s="106"/>
-      <c r="AE26" s="106"/>
-      <c r="AF26" s="106"/>
-      <c r="AG26" s="106"/>
-      <c r="AH26" s="106"/>
-      <c r="AI26" s="106"/>
-      <c r="AJ26" s="107"/>
+      <c r="J26" s="111"/>
+      <c r="K26" s="111"/>
+      <c r="L26" s="111"/>
+      <c r="M26" s="111"/>
+      <c r="N26" s="111"/>
+      <c r="O26" s="111"/>
+      <c r="P26" s="111"/>
+      <c r="Q26" s="111"/>
+      <c r="R26" s="111"/>
+      <c r="S26" s="111"/>
+      <c r="T26" s="111"/>
+      <c r="U26" s="111"/>
+      <c r="V26" s="111"/>
+      <c r="W26" s="111"/>
+      <c r="X26" s="111"/>
+      <c r="Y26" s="111"/>
+      <c r="Z26" s="111"/>
+      <c r="AA26" s="111"/>
+      <c r="AB26" s="111"/>
+      <c r="AC26" s="111"/>
+      <c r="AD26" s="111"/>
+      <c r="AE26" s="111"/>
+      <c r="AF26" s="111"/>
+      <c r="AG26" s="111"/>
+      <c r="AH26" s="111"/>
+      <c r="AI26" s="111"/>
+      <c r="AJ26" s="112"/>
       <c r="AP26" s="8"/>
       <c r="AQ26" s="8"/>
       <c r="AR26" s="8"/>
       <c r="AS26" s="8"/>
     </row>
     <row r="27" spans="2:45" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="116"/>
-      <c r="C27" s="98"/>
-      <c r="D27" s="98"/>
-      <c r="E27" s="98"/>
-      <c r="F27" s="98"/>
-      <c r="G27" s="98"/>
-      <c r="H27" s="100"/>
+      <c r="B27" s="121"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="103"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="105"/>
       <c r="I27" s="25"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
@@ -3865,66 +4173,66 @@
       <c r="AS27" s="8"/>
     </row>
     <row r="28" spans="2:45" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="116"/>
-      <c r="C28" s="98"/>
-      <c r="D28" s="98" t="s">
+      <c r="B28" s="121"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="97" t="s">
+      <c r="E28" s="102" t="s">
         <v>93</v>
       </c>
-      <c r="F28" s="98" t="s">
+      <c r="F28" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="G28" s="98" t="s">
+      <c r="G28" s="103" t="s">
         <v>84</v>
       </c>
-      <c r="H28" s="100" t="s">
+      <c r="H28" s="105" t="s">
         <v>85</v>
       </c>
-      <c r="I28" s="105" t="s">
+      <c r="I28" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="J28" s="106"/>
-      <c r="K28" s="106"/>
-      <c r="L28" s="106"/>
-      <c r="M28" s="106"/>
-      <c r="N28" s="106"/>
-      <c r="O28" s="106"/>
-      <c r="P28" s="106"/>
-      <c r="Q28" s="106"/>
-      <c r="R28" s="106"/>
-      <c r="S28" s="106"/>
-      <c r="T28" s="106"/>
-      <c r="U28" s="106"/>
-      <c r="V28" s="106"/>
-      <c r="W28" s="106"/>
-      <c r="X28" s="106"/>
-      <c r="Y28" s="106"/>
-      <c r="Z28" s="106"/>
-      <c r="AA28" s="106"/>
-      <c r="AB28" s="106"/>
-      <c r="AC28" s="106"/>
-      <c r="AD28" s="106"/>
-      <c r="AE28" s="106"/>
-      <c r="AF28" s="106"/>
-      <c r="AG28" s="106"/>
-      <c r="AH28" s="106"/>
-      <c r="AI28" s="106"/>
-      <c r="AJ28" s="107"/>
+      <c r="J28" s="111"/>
+      <c r="K28" s="111"/>
+      <c r="L28" s="111"/>
+      <c r="M28" s="111"/>
+      <c r="N28" s="111"/>
+      <c r="O28" s="111"/>
+      <c r="P28" s="111"/>
+      <c r="Q28" s="111"/>
+      <c r="R28" s="111"/>
+      <c r="S28" s="111"/>
+      <c r="T28" s="111"/>
+      <c r="U28" s="111"/>
+      <c r="V28" s="111"/>
+      <c r="W28" s="111"/>
+      <c r="X28" s="111"/>
+      <c r="Y28" s="111"/>
+      <c r="Z28" s="111"/>
+      <c r="AA28" s="111"/>
+      <c r="AB28" s="111"/>
+      <c r="AC28" s="111"/>
+      <c r="AD28" s="111"/>
+      <c r="AE28" s="111"/>
+      <c r="AF28" s="111"/>
+      <c r="AG28" s="111"/>
+      <c r="AH28" s="111"/>
+      <c r="AI28" s="111"/>
+      <c r="AJ28" s="112"/>
       <c r="AP28" s="8"/>
       <c r="AQ28" s="8"/>
       <c r="AR28" s="8"/>
       <c r="AS28" s="8"/>
     </row>
     <row r="29" spans="2:45" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="119"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="99"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="99"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="101"/>
+      <c r="B29" s="124"/>
+      <c r="C29" s="104"/>
+      <c r="D29" s="104"/>
+      <c r="E29" s="104"/>
+      <c r="F29" s="104"/>
+      <c r="G29" s="104"/>
+      <c r="H29" s="106"/>
       <c r="I29" s="28"/>
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
@@ -3971,30 +4279,30 @@
       <c r="AS31" s="8"/>
     </row>
     <row r="32" spans="2:45" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="90" t="s">
+      <c r="B32" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="C32" s="91"/>
-      <c r="D32" s="91"/>
-      <c r="E32" s="91"/>
-      <c r="F32" s="91"/>
-      <c r="G32" s="91"/>
-      <c r="H32" s="91"/>
-      <c r="I32" s="91"/>
-      <c r="J32" s="91"/>
-      <c r="K32" s="91"/>
-      <c r="L32" s="91"/>
-      <c r="M32" s="91"/>
-      <c r="N32" s="91"/>
-      <c r="O32" s="91"/>
-      <c r="P32" s="91"/>
-      <c r="Q32" s="91"/>
-      <c r="R32" s="91"/>
-      <c r="S32" s="91"/>
-      <c r="T32" s="91"/>
-      <c r="U32" s="91"/>
-      <c r="V32" s="91"/>
-      <c r="W32" s="92"/>
+      <c r="C32" s="96"/>
+      <c r="D32" s="96"/>
+      <c r="E32" s="96"/>
+      <c r="F32" s="96"/>
+      <c r="G32" s="96"/>
+      <c r="H32" s="96"/>
+      <c r="I32" s="96"/>
+      <c r="J32" s="96"/>
+      <c r="K32" s="96"/>
+      <c r="L32" s="96"/>
+      <c r="M32" s="96"/>
+      <c r="N32" s="96"/>
+      <c r="O32" s="96"/>
+      <c r="P32" s="96"/>
+      <c r="Q32" s="96"/>
+      <c r="R32" s="96"/>
+      <c r="S32" s="96"/>
+      <c r="T32" s="96"/>
+      <c r="U32" s="96"/>
+      <c r="V32" s="96"/>
+      <c r="W32" s="97"/>
     </row>
     <row r="33" spans="2:28" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="29" t="s">
@@ -4023,22 +4331,22 @@
       <c r="W33" s="30"/>
     </row>
     <row r="34" spans="2:28" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="75" t="s">
+      <c r="B34" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
       <c r="E34" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="F34" s="76" t="s">
+      <c r="F34" s="81" t="s">
         <v>120</v>
       </c>
-      <c r="G34" s="76"/>
-      <c r="H34" s="79" t="s">
+      <c r="G34" s="81"/>
+      <c r="H34" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="I34" s="79"/>
+      <c r="I34" s="84"/>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
@@ -4055,18 +4363,18 @@
       <c r="W34" s="30"/>
     </row>
     <row r="35" spans="2:28" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="75" t="s">
+      <c r="B35" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="76"/>
-      <c r="D35" s="76"/>
+      <c r="C35" s="81"/>
+      <c r="D35" s="81"/>
       <c r="E35" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F35" s="76" t="s">
+      <c r="F35" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="G35" s="76"/>
+      <c r="G35" s="81"/>
       <c r="H35" s="38"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
@@ -4085,18 +4393,18 @@
       <c r="W35" s="30"/>
     </row>
     <row r="36" spans="2:28" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="75" t="s">
+      <c r="B36" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="76"/>
-      <c r="D36" s="76"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="81"/>
       <c r="E36" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="F36" s="76" t="s">
+      <c r="F36" s="81" t="s">
         <v>118</v>
       </c>
-      <c r="G36" s="76"/>
+      <c r="G36" s="81"/>
       <c r="H36" s="38"/>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
@@ -4115,32 +4423,32 @@
       <c r="W36" s="30"/>
     </row>
     <row r="37" spans="2:28" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="86" t="s">
+      <c r="B37" s="91" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="87"/>
-      <c r="D37" s="87"/>
-      <c r="E37" s="87"/>
-      <c r="F37" s="87"/>
-      <c r="G37" s="87"/>
-      <c r="H37" s="87"/>
-      <c r="I37" s="87"/>
-      <c r="J37" s="87"/>
-      <c r="K37" s="88" t="s">
+      <c r="C37" s="92"/>
+      <c r="D37" s="92"/>
+      <c r="E37" s="92"/>
+      <c r="F37" s="92"/>
+      <c r="G37" s="92"/>
+      <c r="H37" s="92"/>
+      <c r="I37" s="92"/>
+      <c r="J37" s="92"/>
+      <c r="K37" s="93" t="s">
         <v>128</v>
       </c>
-      <c r="L37" s="88"/>
-      <c r="M37" s="88"/>
-      <c r="N37" s="88"/>
-      <c r="O37" s="88"/>
-      <c r="P37" s="88"/>
-      <c r="Q37" s="88"/>
-      <c r="R37" s="88"/>
-      <c r="S37" s="88"/>
-      <c r="T37" s="88"/>
-      <c r="U37" s="88"/>
-      <c r="V37" s="88"/>
-      <c r="W37" s="89"/>
+      <c r="L37" s="93"/>
+      <c r="M37" s="93"/>
+      <c r="N37" s="93"/>
+      <c r="O37" s="93"/>
+      <c r="P37" s="93"/>
+      <c r="Q37" s="93"/>
+      <c r="R37" s="93"/>
+      <c r="S37" s="93"/>
+      <c r="T37" s="93"/>
+      <c r="U37" s="93"/>
+      <c r="V37" s="93"/>
+      <c r="W37" s="94"/>
       <c r="X37"/>
       <c r="Y37"/>
       <c r="Z37"/>
@@ -4149,23 +4457,23 @@
     </row>
     <row r="38" spans="2:28" customFormat="1" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:28" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="80" t="s">
+      <c r="B39" s="85" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="81"/>
-      <c r="I39" s="81"/>
-      <c r="J39" s="81"/>
-      <c r="K39" s="81"/>
-      <c r="L39" s="81"/>
-      <c r="M39" s="81"/>
-      <c r="N39" s="81"/>
-      <c r="O39" s="81"/>
-      <c r="P39" s="81"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="86"/>
+      <c r="H39" s="86"/>
+      <c r="I39" s="86"/>
+      <c r="J39" s="86"/>
+      <c r="K39" s="86"/>
+      <c r="L39" s="86"/>
+      <c r="M39" s="86"/>
+      <c r="N39" s="86"/>
+      <c r="O39" s="86"/>
+      <c r="P39" s="86"/>
       <c r="Q39" s="33"/>
       <c r="R39" s="33"/>
       <c r="S39" s="33"/>
@@ -4175,48 +4483,48 @@
       <c r="W39" s="34"/>
     </row>
     <row r="40" spans="2:28" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="83" t="s">
+      <c r="B40" s="88" t="s">
         <v>100</v>
       </c>
-      <c r="C40" s="84"/>
-      <c r="D40" s="84"/>
-      <c r="E40" s="84"/>
-      <c r="F40" s="84"/>
-      <c r="G40" s="84"/>
-      <c r="H40" s="84"/>
-      <c r="I40" s="84"/>
-      <c r="J40" s="84"/>
-      <c r="K40" s="84"/>
-      <c r="L40" s="84"/>
-      <c r="M40" s="84"/>
-      <c r="N40" s="84"/>
-      <c r="O40" s="84"/>
-      <c r="P40" s="84"/>
-      <c r="Q40" s="84"/>
-      <c r="R40" s="84"/>
-      <c r="S40" s="84"/>
-      <c r="T40" s="84"/>
-      <c r="U40" s="84"/>
-      <c r="V40" s="84"/>
-      <c r="W40" s="85"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="89"/>
+      <c r="G40" s="89"/>
+      <c r="H40" s="89"/>
+      <c r="I40" s="89"/>
+      <c r="J40" s="89"/>
+      <c r="K40" s="89"/>
+      <c r="L40" s="89"/>
+      <c r="M40" s="89"/>
+      <c r="N40" s="89"/>
+      <c r="O40" s="89"/>
+      <c r="P40" s="89"/>
+      <c r="Q40" s="89"/>
+      <c r="R40" s="89"/>
+      <c r="S40" s="89"/>
+      <c r="T40" s="89"/>
+      <c r="U40" s="89"/>
+      <c r="V40" s="89"/>
+      <c r="W40" s="90"/>
     </row>
     <row r="41" spans="2:28" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="75" t="s">
+      <c r="B41" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="81"/>
       <c r="E41" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="F41" s="76" t="s">
+      <c r="F41" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="G41" s="76"/>
-      <c r="H41" s="79" t="s">
+      <c r="G41" s="81"/>
+      <c r="H41" s="84" t="s">
         <v>103</v>
       </c>
-      <c r="I41" s="79"/>
+      <c r="I41" s="84"/>
       <c r="J41" s="10"/>
       <c r="K41" s="10" t="s">
         <v>122</v>
@@ -4235,18 +4543,18 @@
       <c r="W41" s="30"/>
     </row>
     <row r="42" spans="2:28" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="75" t="s">
+      <c r="B42" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="C42" s="76"/>
-      <c r="D42" s="76"/>
+      <c r="C42" s="81"/>
+      <c r="D42" s="81"/>
       <c r="E42" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F42" s="76" t="s">
+      <c r="F42" s="81" t="s">
         <v>116</v>
       </c>
-      <c r="G42" s="76"/>
+      <c r="G42" s="81"/>
       <c r="H42" s="13"/>
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
@@ -4265,18 +4573,18 @@
       <c r="W42" s="30"/>
     </row>
     <row r="43" spans="2:28" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="77" t="s">
+      <c r="B43" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="C43" s="78"/>
-      <c r="D43" s="78"/>
+      <c r="C43" s="83"/>
+      <c r="D43" s="83"/>
       <c r="E43" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="F43" s="78" t="s">
+      <c r="F43" s="83" t="s">
         <v>117</v>
       </c>
-      <c r="G43" s="78"/>
+      <c r="G43" s="83"/>
       <c r="H43" s="35"/>
       <c r="I43" s="31"/>
       <c r="J43" s="31"/>
@@ -4296,72 +4604,72 @@
     </row>
     <row r="44" spans="2:28" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="45" spans="2:28" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="80" t="s">
+      <c r="B45" s="85" t="s">
         <v>106</v>
       </c>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="81"/>
-      <c r="G45" s="81"/>
-      <c r="H45" s="81"/>
-      <c r="I45" s="81"/>
-      <c r="J45" s="81"/>
-      <c r="K45" s="81"/>
-      <c r="L45" s="81"/>
-      <c r="M45" s="81"/>
-      <c r="N45" s="81"/>
-      <c r="O45" s="81"/>
-      <c r="P45" s="81"/>
-      <c r="Q45" s="81"/>
-      <c r="R45" s="81"/>
-      <c r="S45" s="81"/>
-      <c r="T45" s="81"/>
-      <c r="U45" s="81"/>
-      <c r="V45" s="81"/>
-      <c r="W45" s="82"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
+      <c r="G45" s="86"/>
+      <c r="H45" s="86"/>
+      <c r="I45" s="86"/>
+      <c r="J45" s="86"/>
+      <c r="K45" s="86"/>
+      <c r="L45" s="86"/>
+      <c r="M45" s="86"/>
+      <c r="N45" s="86"/>
+      <c r="O45" s="86"/>
+      <c r="P45" s="86"/>
+      <c r="Q45" s="86"/>
+      <c r="R45" s="86"/>
+      <c r="S45" s="86"/>
+      <c r="T45" s="86"/>
+      <c r="U45" s="86"/>
+      <c r="V45" s="86"/>
+      <c r="W45" s="87"/>
     </row>
     <row r="46" spans="2:28" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="83" t="s">
+      <c r="B46" s="88" t="s">
         <v>109</v>
       </c>
-      <c r="C46" s="84"/>
-      <c r="D46" s="84"/>
-      <c r="E46" s="84"/>
-      <c r="F46" s="84"/>
-      <c r="G46" s="84"/>
-      <c r="H46" s="84"/>
-      <c r="I46" s="84"/>
-      <c r="J46" s="84"/>
-      <c r="K46" s="84"/>
-      <c r="L46" s="84"/>
-      <c r="M46" s="84"/>
-      <c r="N46" s="84"/>
-      <c r="O46" s="84"/>
-      <c r="P46" s="84"/>
-      <c r="Q46" s="84"/>
-      <c r="R46" s="84"/>
-      <c r="S46" s="84"/>
-      <c r="T46" s="84"/>
-      <c r="U46" s="84"/>
-      <c r="V46" s="84"/>
-      <c r="W46" s="85"/>
+      <c r="C46" s="89"/>
+      <c r="D46" s="89"/>
+      <c r="E46" s="89"/>
+      <c r="F46" s="89"/>
+      <c r="G46" s="89"/>
+      <c r="H46" s="89"/>
+      <c r="I46" s="89"/>
+      <c r="J46" s="89"/>
+      <c r="K46" s="89"/>
+      <c r="L46" s="89"/>
+      <c r="M46" s="89"/>
+      <c r="N46" s="89"/>
+      <c r="O46" s="89"/>
+      <c r="P46" s="89"/>
+      <c r="Q46" s="89"/>
+      <c r="R46" s="89"/>
+      <c r="S46" s="89"/>
+      <c r="T46" s="89"/>
+      <c r="U46" s="89"/>
+      <c r="V46" s="89"/>
+      <c r="W46" s="90"/>
     </row>
     <row r="47" spans="2:28" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="75" t="s">
+      <c r="B47" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="76"/>
-      <c r="D47" s="76"/>
+      <c r="C47" s="81"/>
+      <c r="D47" s="81"/>
       <c r="E47" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="84" t="s">
+      <c r="F47" s="89" t="s">
         <v>108</v>
       </c>
-      <c r="G47" s="84"/>
-      <c r="H47" s="84"/>
-      <c r="I47" s="84"/>
+      <c r="G47" s="89"/>
+      <c r="H47" s="89"/>
+      <c r="I47" s="89"/>
       <c r="J47" s="10"/>
       <c r="L47" s="10"/>
       <c r="M47" s="10"/>
@@ -4377,21 +4685,21 @@
       <c r="W47" s="30"/>
     </row>
     <row r="48" spans="2:28" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="75" t="s">
+      <c r="B48" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="76"/>
-      <c r="D48" s="76"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="81"/>
       <c r="E48" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="F48" s="76" t="s">
+      <c r="F48" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="G48" s="76"/>
-      <c r="H48" s="76"/>
-      <c r="I48" s="76"/>
-      <c r="J48" s="76"/>
+      <c r="G48" s="81"/>
+      <c r="H48" s="81"/>
+      <c r="I48" s="81"/>
+      <c r="J48" s="81"/>
       <c r="K48" s="10" t="s">
         <v>123</v>
       </c>
@@ -4433,74 +4741,74 @@
     </row>
     <row r="50" spans="2:23" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="51" spans="2:23" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="80" t="s">
+      <c r="B51" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="C51" s="81"/>
-      <c r="D51" s="81"/>
-      <c r="E51" s="81"/>
-      <c r="F51" s="81"/>
-      <c r="G51" s="81"/>
-      <c r="H51" s="81"/>
-      <c r="I51" s="81"/>
-      <c r="J51" s="81"/>
-      <c r="K51" s="81"/>
-      <c r="L51" s="81"/>
-      <c r="M51" s="81"/>
-      <c r="N51" s="81"/>
-      <c r="O51" s="81"/>
-      <c r="P51" s="81"/>
-      <c r="Q51" s="81"/>
-      <c r="R51" s="81"/>
-      <c r="S51" s="81"/>
-      <c r="T51" s="81"/>
-      <c r="U51" s="81"/>
-      <c r="V51" s="81"/>
-      <c r="W51" s="82"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="86"/>
+      <c r="E51" s="86"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="86"/>
+      <c r="H51" s="86"/>
+      <c r="I51" s="86"/>
+      <c r="J51" s="86"/>
+      <c r="K51" s="86"/>
+      <c r="L51" s="86"/>
+      <c r="M51" s="86"/>
+      <c r="N51" s="86"/>
+      <c r="O51" s="86"/>
+      <c r="P51" s="86"/>
+      <c r="Q51" s="86"/>
+      <c r="R51" s="86"/>
+      <c r="S51" s="86"/>
+      <c r="T51" s="86"/>
+      <c r="U51" s="86"/>
+      <c r="V51" s="86"/>
+      <c r="W51" s="87"/>
     </row>
     <row r="52" spans="2:23" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="83" t="s">
+      <c r="B52" s="88" t="s">
         <v>112</v>
       </c>
-      <c r="C52" s="84"/>
-      <c r="D52" s="84"/>
-      <c r="E52" s="84"/>
-      <c r="F52" s="84"/>
-      <c r="G52" s="84"/>
-      <c r="H52" s="84"/>
-      <c r="I52" s="84"/>
-      <c r="J52" s="84"/>
-      <c r="K52" s="84"/>
-      <c r="L52" s="84"/>
-      <c r="M52" s="84"/>
-      <c r="N52" s="84"/>
-      <c r="O52" s="84"/>
-      <c r="P52" s="84"/>
-      <c r="Q52" s="84"/>
-      <c r="R52" s="84"/>
-      <c r="S52" s="84"/>
-      <c r="T52" s="84"/>
-      <c r="U52" s="84"/>
-      <c r="V52" s="84"/>
-      <c r="W52" s="85"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="89"/>
+      <c r="E52" s="89"/>
+      <c r="F52" s="89"/>
+      <c r="G52" s="89"/>
+      <c r="H52" s="89"/>
+      <c r="I52" s="89"/>
+      <c r="J52" s="89"/>
+      <c r="K52" s="89"/>
+      <c r="L52" s="89"/>
+      <c r="M52" s="89"/>
+      <c r="N52" s="89"/>
+      <c r="O52" s="89"/>
+      <c r="P52" s="89"/>
+      <c r="Q52" s="89"/>
+      <c r="R52" s="89"/>
+      <c r="S52" s="89"/>
+      <c r="T52" s="89"/>
+      <c r="U52" s="89"/>
+      <c r="V52" s="89"/>
+      <c r="W52" s="90"/>
     </row>
     <row r="53" spans="2:23" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="75" t="s">
+      <c r="B53" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="C53" s="76"/>
-      <c r="D53" s="76"/>
+      <c r="C53" s="81"/>
+      <c r="D53" s="81"/>
       <c r="E53" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F53" s="76" t="s">
+      <c r="F53" s="81" t="s">
         <v>119</v>
       </c>
-      <c r="G53" s="76"/>
-      <c r="H53" s="79" t="s">
+      <c r="G53" s="81"/>
+      <c r="H53" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="I53" s="79"/>
+      <c r="I53" s="84"/>
       <c r="J53" s="10"/>
       <c r="K53" s="10" t="s">
         <v>124</v>
@@ -4519,18 +4827,18 @@
       <c r="W53" s="30"/>
     </row>
     <row r="54" spans="2:23" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="77" t="s">
+      <c r="B54" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="78"/>
-      <c r="D54" s="78"/>
+      <c r="C54" s="83"/>
+      <c r="D54" s="83"/>
       <c r="E54" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="F54" s="78" t="s">
+      <c r="F54" s="83" t="s">
         <v>115</v>
       </c>
-      <c r="G54" s="78"/>
+      <c r="G54" s="83"/>
       <c r="H54" s="35"/>
       <c r="I54" s="31"/>
       <c r="J54" s="31"/>
@@ -4650,8 +4958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9743D0A-362D-47CE-80AF-7584D807FC2E}">
   <dimension ref="F5:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4663,80 +4971,80 @@
   <sheetData>
     <row r="5" spans="6:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="6:19" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="78" t="s">
         <v>139</v>
       </c>
-      <c r="G6" s="73"/>
-      <c r="H6" s="120" t="s">
+      <c r="G6" s="78"/>
+      <c r="H6" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="120"/>
-      <c r="J6" s="120"/>
-      <c r="K6" s="120"/>
-      <c r="L6" s="120"/>
-      <c r="M6" s="120"/>
-      <c r="N6" s="120"/>
-      <c r="O6" s="120"/>
-      <c r="P6" s="120"/>
-      <c r="Q6" s="120"/>
-      <c r="R6" s="120"/>
-      <c r="S6" s="120"/>
+      <c r="I6" s="125"/>
+      <c r="J6" s="125"/>
+      <c r="K6" s="125"/>
+      <c r="L6" s="125"/>
+      <c r="M6" s="125"/>
+      <c r="N6" s="125"/>
+      <c r="O6" s="125"/>
+      <c r="P6" s="125"/>
+      <c r="Q6" s="125"/>
+      <c r="R6" s="125"/>
+      <c r="S6" s="125"/>
     </row>
     <row r="7" spans="6:19" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="68" t="s">
+      <c r="F7" s="73" t="s">
         <v>140</v>
       </c>
-      <c r="G7" s="68"/>
-      <c r="H7" s="120" t="s">
+      <c r="G7" s="73"/>
+      <c r="H7" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="120"/>
-      <c r="J7" s="120"/>
-      <c r="K7" s="120"/>
-      <c r="L7" s="120"/>
-      <c r="M7" s="120"/>
-      <c r="N7" s="120"/>
-      <c r="O7" s="120"/>
-      <c r="P7" s="120"/>
-      <c r="Q7" s="120"/>
-      <c r="R7" s="120"/>
-      <c r="S7" s="120"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="125"/>
+      <c r="M7" s="125"/>
+      <c r="N7" s="125"/>
+      <c r="O7" s="125"/>
+      <c r="P7" s="125"/>
+      <c r="Q7" s="125"/>
+      <c r="R7" s="125"/>
+      <c r="S7" s="125"/>
     </row>
     <row r="8" spans="6:19" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="69" t="s">
+      <c r="F8" s="74" t="s">
         <v>141</v>
       </c>
-      <c r="G8" s="69"/>
-      <c r="H8" s="120" t="s">
+      <c r="G8" s="74"/>
+      <c r="H8" s="125" t="s">
         <v>129</v>
       </c>
-      <c r="I8" s="120"/>
-      <c r="J8" s="120"/>
-      <c r="K8" s="120"/>
-      <c r="L8" s="120"/>
-      <c r="M8" s="120"/>
-      <c r="N8" s="120"/>
-      <c r="O8" s="120"/>
-      <c r="P8" s="120"/>
-      <c r="Q8" s="120"/>
-      <c r="R8" s="120"/>
-      <c r="S8" s="120"/>
+      <c r="I8" s="125"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="125"/>
+      <c r="L8" s="125"/>
+      <c r="M8" s="125"/>
+      <c r="N8" s="125"/>
+      <c r="O8" s="125"/>
+      <c r="P8" s="125"/>
+      <c r="Q8" s="125"/>
+      <c r="R8" s="125"/>
+      <c r="S8" s="125"/>
     </row>
     <row r="9" spans="6:19" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="6:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="6:19" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F12" s="134" t="s">
+      <c r="F12" s="140" t="s">
         <v>147</v>
       </c>
-      <c r="G12" s="135"/>
-      <c r="H12" s="135"/>
-      <c r="I12" s="135"/>
-      <c r="J12" s="135"/>
-      <c r="K12" s="135"/>
-      <c r="L12" s="135"/>
-      <c r="M12" s="135"/>
-      <c r="N12" s="135"/>
-      <c r="O12" s="136"/>
+      <c r="G12" s="141"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="141"/>
+      <c r="J12" s="141"/>
+      <c r="K12" s="141"/>
+      <c r="L12" s="141"/>
+      <c r="M12" s="141"/>
+      <c r="N12" s="141"/>
+      <c r="O12" s="142"/>
     </row>
     <row r="13" spans="6:19" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F13" s="43"/>
@@ -4753,64 +5061,64 @@
     <row r="14" spans="6:19" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F14" s="43"/>
       <c r="G14" s="45"/>
-      <c r="H14" s="122" t="s">
+      <c r="H14" s="127" t="s">
         <v>131</v>
       </c>
-      <c r="I14" s="122"/>
-      <c r="J14" s="122" t="s">
+      <c r="I14" s="127"/>
+      <c r="J14" s="127" t="s">
         <v>130</v>
       </c>
-      <c r="K14" s="122"/>
-      <c r="L14" s="122" t="s">
+      <c r="K14" s="127"/>
+      <c r="L14" s="127" t="s">
         <v>145</v>
       </c>
-      <c r="M14" s="122"/>
-      <c r="N14" s="122" t="s">
+      <c r="M14" s="127"/>
+      <c r="N14" s="127" t="s">
         <v>146</v>
       </c>
-      <c r="O14" s="122"/>
+      <c r="O14" s="127"/>
     </row>
     <row r="15" spans="6:19" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F15" s="127" t="s">
+      <c r="F15" s="132" t="s">
         <v>158</v>
       </c>
-      <c r="G15" s="128"/>
-      <c r="H15" s="123" t="s">
+      <c r="G15" s="133"/>
+      <c r="H15" s="128" t="s">
         <v>154</v>
       </c>
-      <c r="I15" s="124"/>
-      <c r="J15" s="124" t="s">
+      <c r="I15" s="129"/>
+      <c r="J15" s="129" t="s">
         <v>148</v>
       </c>
-      <c r="K15" s="124"/>
-      <c r="L15" s="124" t="s">
+      <c r="K15" s="129"/>
+      <c r="L15" s="129" t="s">
         <v>165</v>
       </c>
-      <c r="M15" s="124"/>
-      <c r="N15" s="124" t="s">
+      <c r="M15" s="129"/>
+      <c r="N15" s="129" t="s">
         <v>166</v>
       </c>
-      <c r="O15" s="139"/>
+      <c r="O15" s="145"/>
     </row>
     <row r="16" spans="6:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F16" s="129"/>
-      <c r="G16" s="130"/>
-      <c r="H16" s="137" t="s">
+      <c r="F16" s="134"/>
+      <c r="G16" s="135"/>
+      <c r="H16" s="143" t="s">
         <v>155</v>
       </c>
-      <c r="I16" s="138"/>
-      <c r="J16" s="138" t="s">
+      <c r="I16" s="144"/>
+      <c r="J16" s="144" t="s">
         <v>149</v>
       </c>
-      <c r="K16" s="138"/>
-      <c r="L16" s="138" t="s">
+      <c r="K16" s="144"/>
+      <c r="L16" s="144" t="s">
         <v>151</v>
       </c>
-      <c r="M16" s="138"/>
-      <c r="N16" s="138" t="s">
+      <c r="M16" s="144"/>
+      <c r="N16" s="144" t="s">
         <v>156</v>
       </c>
-      <c r="O16" s="140"/>
+      <c r="O16" s="146"/>
     </row>
     <row r="17" spans="6:21" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F17" s="47"/>
@@ -4823,136 +5131,136 @@
       <c r="O17" s="46"/>
     </row>
     <row r="18" spans="6:21" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="131" t="s">
+      <c r="F18" s="136" t="s">
         <v>144</v>
       </c>
-      <c r="G18" s="132"/>
-      <c r="H18" s="132"/>
-      <c r="I18" s="132"/>
-      <c r="J18" s="132"/>
-      <c r="K18" s="132"/>
-      <c r="L18" s="132"/>
-      <c r="M18" s="132"/>
-      <c r="N18" s="132"/>
-      <c r="O18" s="133"/>
+      <c r="G18" s="137"/>
+      <c r="H18" s="137"/>
+      <c r="I18" s="137"/>
+      <c r="J18" s="137"/>
+      <c r="K18" s="137"/>
+      <c r="L18" s="137"/>
+      <c r="M18" s="137"/>
+      <c r="N18" s="137"/>
+      <c r="O18" s="138"/>
     </row>
     <row r="19" spans="6:21" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="40"/>
       <c r="G19" s="42"/>
-      <c r="H19" s="122" t="s">
+      <c r="H19" s="127" t="s">
         <v>131</v>
       </c>
-      <c r="I19" s="122"/>
-      <c r="J19" s="122" t="s">
+      <c r="I19" s="127"/>
+      <c r="J19" s="127" t="s">
         <v>130</v>
       </c>
-      <c r="K19" s="122"/>
-      <c r="L19" s="122" t="s">
+      <c r="K19" s="127"/>
+      <c r="L19" s="127" t="s">
         <v>145</v>
       </c>
-      <c r="M19" s="122"/>
-      <c r="N19" s="122" t="s">
+      <c r="M19" s="127"/>
+      <c r="N19" s="127" t="s">
         <v>146</v>
       </c>
-      <c r="O19" s="122"/>
+      <c r="O19" s="127"/>
     </row>
     <row r="20" spans="6:21" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F20" s="141" t="s">
+      <c r="F20" s="147" t="s">
         <v>134</v>
       </c>
-      <c r="G20" s="141"/>
-      <c r="H20" s="123" t="s">
+      <c r="G20" s="147"/>
+      <c r="H20" s="128" t="s">
         <v>137</v>
       </c>
-      <c r="I20" s="124"/>
-      <c r="J20" s="124" t="s">
+      <c r="I20" s="129"/>
+      <c r="J20" s="129" t="s">
         <v>142</v>
       </c>
-      <c r="K20" s="124"/>
-      <c r="L20" s="124" t="s">
+      <c r="K20" s="129"/>
+      <c r="L20" s="129" t="s">
         <v>150</v>
       </c>
-      <c r="M20" s="124"/>
-      <c r="N20" s="124" t="s">
+      <c r="M20" s="129"/>
+      <c r="N20" s="129" t="s">
         <v>167</v>
       </c>
-      <c r="O20" s="139"/>
-      <c r="P20" s="125" t="s">
+      <c r="O20" s="145"/>
+      <c r="P20" s="130" t="s">
         <v>169</v>
       </c>
-      <c r="Q20" s="126"/>
-      <c r="R20" s="126"/>
-      <c r="S20" s="126"/>
-      <c r="T20" s="126"/>
-      <c r="U20" s="126"/>
+      <c r="Q20" s="131"/>
+      <c r="R20" s="131"/>
+      <c r="S20" s="131"/>
+      <c r="T20" s="131"/>
+      <c r="U20" s="131"/>
     </row>
     <row r="21" spans="6:21" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F21" s="141"/>
-      <c r="G21" s="141"/>
-      <c r="H21" s="137" t="s">
+      <c r="F21" s="147"/>
+      <c r="G21" s="147"/>
+      <c r="H21" s="143" t="s">
         <v>143</v>
       </c>
-      <c r="I21" s="138"/>
-      <c r="J21" s="138" t="s">
+      <c r="I21" s="144"/>
+      <c r="J21" s="144" t="s">
         <v>157</v>
       </c>
-      <c r="K21" s="138"/>
-      <c r="L21" s="138" t="s">
+      <c r="K21" s="144"/>
+      <c r="L21" s="144" t="s">
         <v>152</v>
       </c>
-      <c r="M21" s="138"/>
-      <c r="N21" s="138" t="s">
+      <c r="M21" s="144"/>
+      <c r="N21" s="144" t="s">
         <v>168</v>
       </c>
-      <c r="O21" s="140"/>
-      <c r="P21" s="125" t="s">
+      <c r="O21" s="146"/>
+      <c r="P21" s="130" t="s">
         <v>170</v>
       </c>
-      <c r="Q21" s="126"/>
-      <c r="R21" s="126"/>
-      <c r="S21" s="126"/>
-      <c r="T21" s="126"/>
-      <c r="U21" s="126"/>
+      <c r="Q21" s="131"/>
+      <c r="R21" s="131"/>
+      <c r="S21" s="131"/>
+      <c r="T21" s="131"/>
+      <c r="U21" s="131"/>
     </row>
     <row r="22" spans="6:21" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="F22" s="39"/>
       <c r="G22" s="39"/>
     </row>
     <row r="24" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="K24" s="121" t="s">
+      <c r="K24" s="126" t="s">
         <v>163</v>
       </c>
-      <c r="L24" s="121"/>
-      <c r="M24" s="121"/>
-      <c r="N24" s="121"/>
-      <c r="O24" s="121"/>
-      <c r="P24" s="121"/>
-      <c r="Q24" s="121"/>
-      <c r="R24" s="121"/>
-      <c r="S24" s="121"/>
-      <c r="T24" s="121"/>
-      <c r="U24" s="121"/>
+      <c r="L24" s="126"/>
+      <c r="M24" s="126"/>
+      <c r="N24" s="126"/>
+      <c r="O24" s="126"/>
+      <c r="P24" s="126"/>
+      <c r="Q24" s="126"/>
+      <c r="R24" s="126"/>
+      <c r="S24" s="126"/>
+      <c r="T24" s="126"/>
+      <c r="U24" s="126"/>
     </row>
     <row r="25" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="F25" s="142" t="s">
+      <c r="F25" s="148" t="s">
         <v>159</v>
       </c>
-      <c r="G25" s="143"/>
-      <c r="H25" s="143"/>
-      <c r="I25" s="144"/>
-      <c r="K25" s="145" t="s">
+      <c r="G25" s="149"/>
+      <c r="H25" s="149"/>
+      <c r="I25" s="150"/>
+      <c r="K25" s="139" t="s">
         <v>160</v>
       </c>
-      <c r="L25" s="145"/>
-      <c r="M25" s="145"/>
-      <c r="N25" s="145"/>
-      <c r="O25" s="145"/>
-      <c r="P25" s="145"/>
-      <c r="Q25" s="145"/>
-      <c r="R25" s="145"/>
-      <c r="S25" s="145"/>
-      <c r="T25" s="145"/>
-      <c r="U25" s="145"/>
+      <c r="L25" s="139"/>
+      <c r="M25" s="139"/>
+      <c r="N25" s="139"/>
+      <c r="O25" s="139"/>
+      <c r="P25" s="139"/>
+      <c r="Q25" s="139"/>
+      <c r="R25" s="139"/>
+      <c r="S25" s="139"/>
+      <c r="T25" s="139"/>
+      <c r="U25" s="139"/>
     </row>
     <row r="26" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F26" s="49"/>
@@ -4963,25 +5271,25 @@
       <c r="I26" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="K26" s="145" t="s">
+      <c r="K26" s="139" t="s">
         <v>161</v>
       </c>
-      <c r="L26" s="145"/>
-      <c r="M26" s="145"/>
-      <c r="N26" s="145"/>
-      <c r="O26" s="145"/>
-      <c r="P26" s="145"/>
-      <c r="Q26" s="145"/>
-      <c r="R26" s="145"/>
-      <c r="S26" s="145"/>
-      <c r="T26" s="145"/>
-      <c r="U26" s="145"/>
+      <c r="L26" s="139"/>
+      <c r="M26" s="139"/>
+      <c r="N26" s="139"/>
+      <c r="O26" s="139"/>
+      <c r="P26" s="139"/>
+      <c r="Q26" s="139"/>
+      <c r="R26" s="139"/>
+      <c r="S26" s="139"/>
+      <c r="T26" s="139"/>
+      <c r="U26" s="139"/>
     </row>
     <row r="27" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="F27" s="121" t="s">
+      <c r="F27" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="121"/>
+      <c r="G27" s="126"/>
       <c r="H27" s="49" t="s">
         <v>136</v>
       </c>
@@ -4989,24 +5297,24 @@
         <v>153</v>
       </c>
       <c r="K27" s="49"/>
-      <c r="L27" s="145" t="s">
+      <c r="L27" s="139" t="s">
         <v>162</v>
       </c>
-      <c r="M27" s="145"/>
-      <c r="N27" s="145"/>
-      <c r="O27" s="145"/>
-      <c r="P27" s="145"/>
-      <c r="Q27" s="145"/>
-      <c r="R27" s="145"/>
-      <c r="S27" s="145"/>
-      <c r="T27" s="145"/>
-      <c r="U27" s="145"/>
+      <c r="M27" s="139"/>
+      <c r="N27" s="139"/>
+      <c r="O27" s="139"/>
+      <c r="P27" s="139"/>
+      <c r="Q27" s="139"/>
+      <c r="R27" s="139"/>
+      <c r="S27" s="139"/>
+      <c r="T27" s="139"/>
+      <c r="U27" s="139"/>
     </row>
     <row r="28" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="F28" s="121" t="s">
+      <c r="F28" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="G28" s="121"/>
+      <c r="G28" s="126"/>
       <c r="H28" s="49" t="s">
         <v>135</v>
       </c>
@@ -5014,33 +5322,33 @@
         <v>138</v>
       </c>
       <c r="K28" s="49"/>
-      <c r="L28" s="145" t="s">
+      <c r="L28" s="139" t="s">
         <v>164</v>
       </c>
-      <c r="M28" s="145"/>
-      <c r="N28" s="145"/>
-      <c r="O28" s="145"/>
-      <c r="P28" s="145"/>
-      <c r="Q28" s="145"/>
-      <c r="R28" s="145"/>
-      <c r="S28" s="145"/>
-      <c r="T28" s="145"/>
-      <c r="U28" s="145"/>
+      <c r="M28" s="139"/>
+      <c r="N28" s="139"/>
+      <c r="O28" s="139"/>
+      <c r="P28" s="139"/>
+      <c r="Q28" s="139"/>
+      <c r="R28" s="139"/>
+      <c r="S28" s="139"/>
+      <c r="T28" s="139"/>
+      <c r="U28" s="139"/>
     </row>
     <row r="30" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="F30" s="126"/>
-      <c r="G30" s="126"/>
-      <c r="H30" s="126"/>
-      <c r="I30" s="126"/>
-      <c r="J30" s="126"/>
-      <c r="K30" s="126"/>
-      <c r="L30" s="126"/>
-      <c r="M30" s="126"/>
-      <c r="N30" s="126"/>
-      <c r="O30" s="126"/>
-      <c r="P30" s="126"/>
-      <c r="Q30" s="126"/>
-      <c r="R30" s="126"/>
+      <c r="F30" s="131"/>
+      <c r="G30" s="131"/>
+      <c r="H30" s="131"/>
+      <c r="I30" s="131"/>
+      <c r="J30" s="131"/>
+      <c r="K30" s="131"/>
+      <c r="L30" s="131"/>
+      <c r="M30" s="131"/>
+      <c r="N30" s="131"/>
+      <c r="O30" s="131"/>
+      <c r="P30" s="131"/>
+      <c r="Q30" s="131"/>
+      <c r="R30" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="45">
@@ -5094,4 +5402,653 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B09D35AF-973D-4939-8501-7A6445A69ABE}">
+  <dimension ref="F5:U56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="18" max="18" width="5.77734375" customWidth="1"/>
+    <col min="19" max="19" width="11.21875" customWidth="1"/>
+    <col min="20" max="20" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="6:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="6:19" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="78" t="s">
+        <v>139</v>
+      </c>
+      <c r="G6" s="78"/>
+      <c r="H6" s="125" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="125"/>
+      <c r="J6" s="125"/>
+      <c r="K6" s="125"/>
+      <c r="L6" s="125"/>
+      <c r="M6" s="125"/>
+      <c r="N6" s="125"/>
+      <c r="O6" s="125"/>
+      <c r="P6" s="125"/>
+      <c r="Q6" s="125"/>
+      <c r="R6" s="125"/>
+      <c r="S6" s="125"/>
+    </row>
+    <row r="7" spans="6:19" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="G7" s="73"/>
+      <c r="H7" s="125" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="125"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="125"/>
+      <c r="M7" s="125"/>
+      <c r="N7" s="125"/>
+      <c r="O7" s="125"/>
+      <c r="P7" s="125"/>
+      <c r="Q7" s="125"/>
+      <c r="R7" s="125"/>
+      <c r="S7" s="125"/>
+    </row>
+    <row r="8" spans="6:19" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="74" t="s">
+        <v>141</v>
+      </c>
+      <c r="G8" s="74"/>
+      <c r="H8" s="125" t="s">
+        <v>129</v>
+      </c>
+      <c r="I8" s="125"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="125"/>
+      <c r="L8" s="125"/>
+      <c r="M8" s="125"/>
+      <c r="N8" s="125"/>
+      <c r="O8" s="125"/>
+      <c r="P8" s="125"/>
+      <c r="Q8" s="125"/>
+      <c r="R8" s="125"/>
+      <c r="S8" s="125"/>
+    </row>
+    <row r="9" spans="6:19" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="U21" s="50"/>
+    </row>
+    <row r="22" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="U22" s="50"/>
+    </row>
+    <row r="24" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="G24" s="151" t="s">
+        <v>196</v>
+      </c>
+      <c r="H24" s="151"/>
+      <c r="I24" s="151"/>
+      <c r="J24" s="151"/>
+      <c r="K24" s="151"/>
+      <c r="L24" s="151"/>
+      <c r="M24" s="151"/>
+    </row>
+    <row r="25" spans="6:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="6:21" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="140" t="s">
+        <v>188</v>
+      </c>
+      <c r="G26" s="141"/>
+      <c r="H26" s="141"/>
+      <c r="I26" s="141"/>
+      <c r="J26" s="141"/>
+      <c r="K26" s="141"/>
+      <c r="L26" s="141"/>
+      <c r="M26" s="141"/>
+      <c r="N26" s="141"/>
+      <c r="O26" s="142"/>
+    </row>
+    <row r="27" spans="6:21" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="168" t="s">
+        <v>171</v>
+      </c>
+      <c r="G27" s="169"/>
+      <c r="H27" s="169"/>
+      <c r="I27" s="169"/>
+      <c r="J27" s="169"/>
+      <c r="K27" s="169"/>
+      <c r="L27" s="169"/>
+      <c r="M27" s="169"/>
+      <c r="N27" s="169"/>
+      <c r="O27" s="170"/>
+      <c r="Q27" s="148" t="s">
+        <v>190</v>
+      </c>
+      <c r="R27" s="149"/>
+      <c r="S27" s="149"/>
+      <c r="T27" s="150"/>
+    </row>
+    <row r="28" spans="6:21" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="132" t="s">
+        <v>173</v>
+      </c>
+      <c r="G28" s="160"/>
+      <c r="H28" s="127" t="s">
+        <v>131</v>
+      </c>
+      <c r="I28" s="127"/>
+      <c r="J28" s="127" t="s">
+        <v>130</v>
+      </c>
+      <c r="K28" s="127"/>
+      <c r="L28" s="127" t="s">
+        <v>145</v>
+      </c>
+      <c r="M28" s="127"/>
+      <c r="N28" s="127" t="s">
+        <v>146</v>
+      </c>
+      <c r="O28" s="127"/>
+      <c r="Q28" s="148"/>
+      <c r="R28" s="150"/>
+      <c r="S28" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="T28" s="49" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="6:21" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="161"/>
+      <c r="G29" s="162"/>
+      <c r="H29" s="152" t="s">
+        <v>200</v>
+      </c>
+      <c r="I29" s="153"/>
+      <c r="J29" s="156" t="s">
+        <v>194</v>
+      </c>
+      <c r="K29" s="153"/>
+      <c r="L29" s="156" t="s">
+        <v>195</v>
+      </c>
+      <c r="M29" s="153"/>
+      <c r="N29" s="156" t="s">
+        <v>199</v>
+      </c>
+      <c r="O29" s="158"/>
+      <c r="Q29" s="148" t="s">
+        <v>55</v>
+      </c>
+      <c r="R29" s="150"/>
+      <c r="S29" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="T29" s="54" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30" spans="6:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="163"/>
+      <c r="G30" s="164"/>
+      <c r="H30" s="154"/>
+      <c r="I30" s="155"/>
+      <c r="J30" s="157"/>
+      <c r="K30" s="155"/>
+      <c r="L30" s="157"/>
+      <c r="M30" s="155"/>
+      <c r="N30" s="157"/>
+      <c r="O30" s="159"/>
+      <c r="Q30" s="126" t="s">
+        <v>48</v>
+      </c>
+      <c r="R30" s="126"/>
+      <c r="S30" s="54" t="s">
+        <v>193</v>
+      </c>
+      <c r="T30" s="54" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="6:21" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="6:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="6:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="136" t="s">
+        <v>188</v>
+      </c>
+      <c r="G34" s="137"/>
+      <c r="H34" s="137"/>
+      <c r="I34" s="137"/>
+      <c r="J34" s="137"/>
+      <c r="K34" s="137"/>
+      <c r="L34" s="137"/>
+      <c r="M34" s="137"/>
+      <c r="N34" s="137"/>
+      <c r="O34" s="138"/>
+      <c r="Q34" s="148" t="s">
+        <v>181</v>
+      </c>
+      <c r="R34" s="149"/>
+      <c r="S34" s="149"/>
+      <c r="T34" s="150"/>
+    </row>
+    <row r="35" spans="6:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="G35" s="137"/>
+      <c r="H35" s="137"/>
+      <c r="I35" s="137"/>
+      <c r="J35" s="137"/>
+      <c r="K35" s="137"/>
+      <c r="L35" s="137"/>
+      <c r="M35" s="137"/>
+      <c r="N35" s="137"/>
+      <c r="O35" s="138"/>
+      <c r="Q35" s="165" t="s">
+        <v>179</v>
+      </c>
+      <c r="R35" s="166"/>
+      <c r="S35" s="166"/>
+      <c r="T35" s="167"/>
+    </row>
+    <row r="36" spans="6:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="132" t="s">
+        <v>173</v>
+      </c>
+      <c r="G36" s="160"/>
+      <c r="H36" s="168" t="s">
+        <v>174</v>
+      </c>
+      <c r="I36" s="169"/>
+      <c r="J36" s="169"/>
+      <c r="K36" s="170"/>
+      <c r="L36" s="168" t="s">
+        <v>175</v>
+      </c>
+      <c r="M36" s="169"/>
+      <c r="N36" s="169"/>
+      <c r="O36" s="170"/>
+      <c r="Q36" s="165" t="s">
+        <v>180</v>
+      </c>
+      <c r="R36" s="166"/>
+      <c r="S36" s="166"/>
+      <c r="T36" s="167"/>
+    </row>
+    <row r="37" spans="6:20" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F37" s="161"/>
+      <c r="G37" s="162"/>
+      <c r="H37" s="152" t="s">
+        <v>177</v>
+      </c>
+      <c r="I37" s="171"/>
+      <c r="J37" s="171"/>
+      <c r="K37" s="153"/>
+      <c r="L37" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="M37" s="171"/>
+      <c r="N37" s="171"/>
+      <c r="O37" s="158"/>
+      <c r="Q37" s="165" t="s">
+        <v>178</v>
+      </c>
+      <c r="R37" s="166"/>
+      <c r="S37" s="166"/>
+      <c r="T37" s="167"/>
+    </row>
+    <row r="38" spans="6:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F38" s="163"/>
+      <c r="G38" s="164"/>
+      <c r="H38" s="154"/>
+      <c r="I38" s="172"/>
+      <c r="J38" s="172"/>
+      <c r="K38" s="155"/>
+      <c r="L38" s="157"/>
+      <c r="M38" s="172"/>
+      <c r="N38" s="172"/>
+      <c r="O38" s="159"/>
+      <c r="Q38" s="165" t="s">
+        <v>185</v>
+      </c>
+      <c r="R38" s="166"/>
+      <c r="S38" s="166"/>
+      <c r="T38" s="167"/>
+    </row>
+    <row r="39" spans="6:20" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F40" s="52"/>
+    </row>
+    <row r="41" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="G41" s="151" t="s">
+        <v>197</v>
+      </c>
+      <c r="H41" s="151"/>
+      <c r="I41" s="151"/>
+      <c r="J41" s="151"/>
+      <c r="K41" s="151"/>
+      <c r="L41" s="151"/>
+      <c r="M41" s="151"/>
+    </row>
+    <row r="42" spans="6:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="6:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F43" s="140" t="s">
+        <v>189</v>
+      </c>
+      <c r="G43" s="141"/>
+      <c r="H43" s="141"/>
+      <c r="I43" s="141"/>
+      <c r="J43" s="141"/>
+      <c r="K43" s="141"/>
+      <c r="L43" s="141"/>
+      <c r="M43" s="141"/>
+      <c r="N43" s="141"/>
+      <c r="O43" s="142"/>
+    </row>
+    <row r="44" spans="6:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F44" s="168" t="s">
+        <v>171</v>
+      </c>
+      <c r="G44" s="169"/>
+      <c r="H44" s="169"/>
+      <c r="I44" s="169"/>
+      <c r="J44" s="169"/>
+      <c r="K44" s="169"/>
+      <c r="L44" s="169"/>
+      <c r="M44" s="169"/>
+      <c r="N44" s="169"/>
+      <c r="O44" s="170"/>
+      <c r="Q44" s="148" t="s">
+        <v>159</v>
+      </c>
+      <c r="R44" s="149"/>
+      <c r="S44" s="149"/>
+      <c r="T44" s="150"/>
+    </row>
+    <row r="45" spans="6:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F45" s="132" t="s">
+        <v>173</v>
+      </c>
+      <c r="G45" s="160"/>
+      <c r="H45" s="127" t="s">
+        <v>131</v>
+      </c>
+      <c r="I45" s="127"/>
+      <c r="J45" s="127" t="s">
+        <v>130</v>
+      </c>
+      <c r="K45" s="127"/>
+      <c r="L45" s="127" t="s">
+        <v>145</v>
+      </c>
+      <c r="M45" s="127"/>
+      <c r="N45" s="127" t="s">
+        <v>146</v>
+      </c>
+      <c r="O45" s="127"/>
+      <c r="Q45" s="148"/>
+      <c r="R45" s="150"/>
+      <c r="S45" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="T45" s="49" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="6:20" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F46" s="161"/>
+      <c r="G46" s="162"/>
+      <c r="H46" s="128" t="s">
+        <v>154</v>
+      </c>
+      <c r="I46" s="129"/>
+      <c r="J46" s="129" t="s">
+        <v>148</v>
+      </c>
+      <c r="K46" s="129"/>
+      <c r="L46" s="129" t="s">
+        <v>165</v>
+      </c>
+      <c r="M46" s="129"/>
+      <c r="N46" s="129" t="s">
+        <v>166</v>
+      </c>
+      <c r="O46" s="145"/>
+      <c r="Q46" s="148" t="s">
+        <v>55</v>
+      </c>
+      <c r="R46" s="150"/>
+      <c r="S46" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="T46" s="54" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="47" spans="6:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F47" s="163"/>
+      <c r="G47" s="164"/>
+      <c r="H47" s="143" t="s">
+        <v>155</v>
+      </c>
+      <c r="I47" s="144"/>
+      <c r="J47" s="144" t="s">
+        <v>149</v>
+      </c>
+      <c r="K47" s="144"/>
+      <c r="L47" s="144" t="s">
+        <v>151</v>
+      </c>
+      <c r="M47" s="144"/>
+      <c r="N47" s="144" t="s">
+        <v>156</v>
+      </c>
+      <c r="O47" s="146"/>
+      <c r="Q47" s="126" t="s">
+        <v>48</v>
+      </c>
+      <c r="R47" s="126"/>
+      <c r="S47" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="T47" s="54" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="6:20" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="6:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="6:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F51" s="136" t="s">
+        <v>189</v>
+      </c>
+      <c r="G51" s="137"/>
+      <c r="H51" s="137"/>
+      <c r="I51" s="137"/>
+      <c r="J51" s="137"/>
+      <c r="K51" s="137"/>
+      <c r="L51" s="137"/>
+      <c r="M51" s="137"/>
+      <c r="N51" s="137"/>
+      <c r="O51" s="138"/>
+      <c r="Q51" s="148" t="s">
+        <v>182</v>
+      </c>
+      <c r="R51" s="149"/>
+      <c r="S51" s="149"/>
+      <c r="T51" s="150"/>
+    </row>
+    <row r="52" spans="6:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F52" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="G52" s="137"/>
+      <c r="H52" s="137"/>
+      <c r="I52" s="137"/>
+      <c r="J52" s="137"/>
+      <c r="K52" s="137"/>
+      <c r="L52" s="137"/>
+      <c r="M52" s="137"/>
+      <c r="N52" s="137"/>
+      <c r="O52" s="138"/>
+      <c r="Q52" s="165" t="s">
+        <v>179</v>
+      </c>
+      <c r="R52" s="166"/>
+      <c r="S52" s="166"/>
+      <c r="T52" s="167"/>
+    </row>
+    <row r="53" spans="6:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F53" s="132" t="s">
+        <v>173</v>
+      </c>
+      <c r="G53" s="160"/>
+      <c r="H53" s="168" t="s">
+        <v>174</v>
+      </c>
+      <c r="I53" s="169"/>
+      <c r="J53" s="169"/>
+      <c r="K53" s="169"/>
+      <c r="L53" s="169"/>
+      <c r="M53" s="169"/>
+      <c r="N53" s="169"/>
+      <c r="O53" s="170"/>
+      <c r="Q53" s="165" t="s">
+        <v>183</v>
+      </c>
+      <c r="R53" s="166"/>
+      <c r="S53" s="166"/>
+      <c r="T53" s="167"/>
+    </row>
+    <row r="54" spans="6:20" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F54" s="161"/>
+      <c r="G54" s="162"/>
+      <c r="H54" s="152" t="s">
+        <v>187</v>
+      </c>
+      <c r="I54" s="171"/>
+      <c r="J54" s="171"/>
+      <c r="K54" s="171"/>
+      <c r="L54" s="171"/>
+      <c r="M54" s="171"/>
+      <c r="N54" s="171"/>
+      <c r="O54" s="158"/>
+      <c r="Q54" s="165" t="s">
+        <v>184</v>
+      </c>
+      <c r="R54" s="166"/>
+      <c r="S54" s="166"/>
+      <c r="T54" s="167"/>
+    </row>
+    <row r="55" spans="6:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F55" s="163"/>
+      <c r="G55" s="164"/>
+      <c r="H55" s="154"/>
+      <c r="I55" s="172"/>
+      <c r="J55" s="172"/>
+      <c r="K55" s="172"/>
+      <c r="L55" s="172"/>
+      <c r="M55" s="172"/>
+      <c r="N55" s="172"/>
+      <c r="O55" s="159"/>
+      <c r="Q55" s="165" t="s">
+        <v>186</v>
+      </c>
+      <c r="R55" s="166"/>
+      <c r="S55" s="166"/>
+      <c r="T55" s="167"/>
+    </row>
+    <row r="56" spans="6:20" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F56" s="53"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="53"/>
+      <c r="J56" s="53"/>
+      <c r="K56" s="53"/>
+      <c r="L56" s="53"/>
+      <c r="M56" s="53"/>
+      <c r="N56" s="53"/>
+      <c r="O56" s="53"/>
+      <c r="P56" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="64">
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:S6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:S7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:S8"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="F43:O43"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="H53:O53"/>
+    <mergeCell ref="F45:G47"/>
+    <mergeCell ref="F36:G38"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="F34:O34"/>
+    <mergeCell ref="F35:O35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K38"/>
+    <mergeCell ref="L36:O36"/>
+    <mergeCell ref="L37:O38"/>
+    <mergeCell ref="F44:O44"/>
+    <mergeCell ref="Q44:T44"/>
+    <mergeCell ref="Q46:R46"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="Q34:T34"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="F53:G55"/>
+    <mergeCell ref="F52:O52"/>
+    <mergeCell ref="F51:O51"/>
+    <mergeCell ref="Q55:T55"/>
+    <mergeCell ref="F26:O26"/>
+    <mergeCell ref="F27:O27"/>
+    <mergeCell ref="F28:G30"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="H54:O55"/>
+    <mergeCell ref="Q51:T51"/>
+    <mergeCell ref="Q52:T52"/>
+    <mergeCell ref="Q53:T53"/>
+    <mergeCell ref="Q54:T54"/>
+    <mergeCell ref="G24:M24"/>
+    <mergeCell ref="G41:M41"/>
+    <mergeCell ref="Q27:T27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="H29:I30"/>
+    <mergeCell ref="J29:K30"/>
+    <mergeCell ref="L29:M30"/>
+    <mergeCell ref="N29:O30"/>
+    <mergeCell ref="Q38:T38"/>
+    <mergeCell ref="Q35:T35"/>
+    <mergeCell ref="Q36:T36"/>
+    <mergeCell ref="Q37:T37"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>